<commit_message>
excel con bus occupatuon
</commit_message>
<xml_diff>
--- a/Schemes/Variables_Lifetime.xlsx
+++ b/Schemes/Variables_Lifetime.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\skipi\Desktop\Leo\PoliTo\Anno4\Semestre1\SDI\FFT_OpSanSilvestro_2025-2026\Schemes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{757B4EE6-24FB-465A-ABF3-5ECF99724B11}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A66AD8E-B33F-433C-A236-8A4B55884A46}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="12975" tabRatio="500" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1384" uniqueCount="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1383" uniqueCount="130">
   <si>
     <t>AR</t>
   </si>
@@ -312,6 +312,114 @@
   <si>
     <t>reg5(A'I) =&gt; OUT0</t>
   </si>
+  <si>
+    <t>RAR</t>
+  </si>
+  <si>
+    <t>RAI</t>
+  </si>
+  <si>
+    <t>IN1(BR) =&gt; reg0</t>
+  </si>
+  <si>
+    <t>IN1(BI) =&gt;reg1</t>
+  </si>
+  <si>
+    <t>AB(WRxBR) =&gt;reg1</t>
+  </si>
+  <si>
+    <t>AB(WIxBI) =&gt;reg1</t>
+  </si>
+  <si>
+    <t>AB(WRxBI)=&gt; reg1</t>
+  </si>
+  <si>
+    <t>AB(WIxBR)=&gt;reg1</t>
+  </si>
+  <si>
+    <t>AB(WRxBI) =&gt; reg1</t>
+  </si>
+  <si>
+    <t>SUM(S1) =&gt; RS</t>
+  </si>
+  <si>
+    <t>SUM(S4) =&gt; RS</t>
+  </si>
+  <si>
+    <t>2A(2AR) =&gt; reg2</t>
+  </si>
+  <si>
+    <t>R(A'R) =&gt; reg2</t>
+  </si>
+  <si>
+    <t>2A(2AI)=&gt;reg3</t>
+  </si>
+  <si>
+    <t>R(A'I)=&gt; reg3</t>
+  </si>
+  <si>
+    <t>R(B'R)=&gt;reg0</t>
+  </si>
+  <si>
+    <t>R(B'I)=&gt;reg2</t>
+  </si>
+  <si>
+    <t>reg0(BR) =&gt;B</t>
+  </si>
+  <si>
+    <t>reg1(BI) =&gt;B</t>
+  </si>
+  <si>
+    <t>reg1(BI)=&gt;B</t>
+  </si>
+  <si>
+    <t>reg1(WIxBI) =&gt; BSUB</t>
+  </si>
+  <si>
+    <t>reg1(WIxBR)=&gt;BSUM</t>
+  </si>
+  <si>
+    <t>reg2(2AR) = ASUB</t>
+  </si>
+  <si>
+    <t>reg3(2AI) = ASUB</t>
+  </si>
+  <si>
+    <t>reg1(WRxBR) =&gt; BSUM</t>
+  </si>
+  <si>
+    <t>reg0(BR)=&gt;B</t>
+  </si>
+  <si>
+    <t>reg0(B'R) =&gt; OUT1</t>
+  </si>
+  <si>
+    <t>reg2(A'R) =&gt; OUT0</t>
+  </si>
+  <si>
+    <t>reg2(B'I) =&gt; OUT1</t>
+  </si>
+  <si>
+    <t>reg3(A'I) =&gt; OUT0</t>
+  </si>
+  <si>
+    <t>RS(S1) =&gt; ASUB</t>
+  </si>
+  <si>
+    <t>RS(S4) =&gt; ASUM</t>
+  </si>
+  <si>
+    <t>RS(S2) =&gt; ASUM</t>
+  </si>
+  <si>
+    <t>RS(S5) =&gt; ASUM</t>
+  </si>
+  <si>
+    <t>IN0 (AR) =&gt; RAR</t>
+  </si>
+  <si>
+    <t>IN0(AI) =&gt;RAI</t>
+  </si>
 </sst>
 </file>
 
@@ -340,7 +448,7 @@
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="21">
+  <fills count="22">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -458,6 +566,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.39997558519241921"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1150,7 +1264,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="128">
+  <cellXfs count="130">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1501,6 +1615,8 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="15" borderId="37" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="15" borderId="52" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="21" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="21" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normale" xfId="0" builtinId="0"/>
@@ -3998,13 +4114,13 @@
     <xdr:from>
       <xdr:col>4</xdr:col>
       <xdr:colOff>346089</xdr:colOff>
-      <xdr:row>69</xdr:row>
+      <xdr:row>73</xdr:row>
       <xdr:rowOff>119212</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
       <xdr:colOff>524011</xdr:colOff>
-      <xdr:row>70</xdr:row>
+      <xdr:row>74</xdr:row>
       <xdr:rowOff>28345</xdr:rowOff>
     </xdr:to>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
@@ -4063,13 +4179,13 @@
     <xdr:from>
       <xdr:col>5</xdr:col>
       <xdr:colOff>442702</xdr:colOff>
-      <xdr:row>69</xdr:row>
+      <xdr:row>73</xdr:row>
       <xdr:rowOff>92932</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
       <xdr:colOff>447824</xdr:colOff>
-      <xdr:row>69</xdr:row>
+      <xdr:row>73</xdr:row>
       <xdr:rowOff>93292</xdr:rowOff>
     </xdr:to>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
@@ -4128,13 +4244,13 @@
     <xdr:from>
       <xdr:col>3</xdr:col>
       <xdr:colOff>775435</xdr:colOff>
-      <xdr:row>75</xdr:row>
+      <xdr:row>73</xdr:row>
       <xdr:rowOff>46924</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
       <xdr:colOff>100517</xdr:colOff>
-      <xdr:row>76</xdr:row>
+      <xdr:row>74</xdr:row>
       <xdr:rowOff>77677</xdr:rowOff>
     </xdr:to>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
@@ -4193,13 +4309,13 @@
     <xdr:from>
       <xdr:col>4</xdr:col>
       <xdr:colOff>372729</xdr:colOff>
-      <xdr:row>75</xdr:row>
+      <xdr:row>73</xdr:row>
       <xdr:rowOff>6244</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
       <xdr:colOff>532929</xdr:colOff>
-      <xdr:row>75</xdr:row>
+      <xdr:row>73</xdr:row>
       <xdr:rowOff>113164</xdr:rowOff>
     </xdr:to>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
@@ -4258,14 +4374,14 @@
     <xdr:from>
       <xdr:col>6</xdr:col>
       <xdr:colOff>12996</xdr:colOff>
-      <xdr:row>74</xdr:row>
+      <xdr:row>78</xdr:row>
       <xdr:rowOff>103372</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
       <xdr:colOff>197758</xdr:colOff>
-      <xdr:row>75</xdr:row>
-      <xdr:rowOff>94167</xdr:rowOff>
+      <xdr:row>79</xdr:row>
+      <xdr:rowOff>94168</xdr:rowOff>
     </xdr:to>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
       <mc:Choice Requires="xdr14">
@@ -4322,84 +4438,19 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>702396</xdr:colOff>
-      <xdr:row>74</xdr:row>
-      <xdr:rowOff>72412</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>158915</xdr:colOff>
-      <xdr:row>75</xdr:row>
-      <xdr:rowOff>77165</xdr:rowOff>
-    </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
-      <mc:Choice Requires="xdr14">
-        <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId13">
-          <xdr14:nvContentPartPr>
-            <xdr14:cNvPr id="7" name="Input penna 6">
-              <a:extLst>
-                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{40064B04-CCE6-438F-A4BE-A0202D757A95}"/>
-                </a:ext>
-              </a:extLst>
-            </xdr14:cNvPr>
-            <xdr14:cNvContentPartPr/>
-          </xdr14:nvContentPartPr>
-          <xdr14:nvPr macro=""/>
-          <xdr14:xfrm>
-            <a:off x="7196714" y="13533968"/>
-            <a:ext cx="218520" cy="147960"/>
-          </xdr14:xfrm>
-        </xdr:contentPart>
-      </mc:Choice>
-      <mc:Fallback xmlns="">
-        <xdr:pic>
-          <xdr:nvPicPr>
-            <xdr:cNvPr id="18" name="Input penna 17">
-              <a:extLst>
-                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{858A1CA8-7109-C499-134E-F8F88DF5326D}"/>
-                </a:ext>
-              </a:extLst>
-            </xdr:cNvPr>
-            <xdr:cNvPicPr/>
-          </xdr:nvPicPr>
-          <xdr:blipFill>
-            <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId14"/>
-            <a:stretch>
-              <a:fillRect/>
-            </a:stretch>
-          </xdr:blipFill>
-          <xdr:spPr>
-            <a:xfrm>
-              <a:off x="7190594" y="13527833"/>
-              <a:ext cx="230760" cy="160230"/>
-            </a:xfrm>
-            <a:prstGeom prst="rect">
-              <a:avLst/>
-            </a:prstGeom>
-          </xdr:spPr>
-        </xdr:pic>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>6</xdr:col>
       <xdr:colOff>283015</xdr:colOff>
-      <xdr:row>86</xdr:row>
+      <xdr:row>84</xdr:row>
       <xdr:rowOff>36556</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
       <xdr:colOff>475615</xdr:colOff>
-      <xdr:row>87</xdr:row>
+      <xdr:row>85</xdr:row>
       <xdr:rowOff>49586</xdr:rowOff>
     </xdr:to>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
       <mc:Choice Requires="xdr14">
-        <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId15">
+        <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId13">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="8" name="Input penna 7">
               <a:extLst>
@@ -4453,13 +4504,13 @@
     <xdr:from>
       <xdr:col>9</xdr:col>
       <xdr:colOff>425909</xdr:colOff>
-      <xdr:row>82</xdr:row>
+      <xdr:row>80</xdr:row>
       <xdr:rowOff>125875</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
       <xdr:colOff>504471</xdr:colOff>
-      <xdr:row>83</xdr:row>
+      <xdr:row>81</xdr:row>
       <xdr:rowOff>77797</xdr:rowOff>
     </xdr:to>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
@@ -4518,13 +4569,13 @@
     <xdr:from>
       <xdr:col>5</xdr:col>
       <xdr:colOff>592498</xdr:colOff>
-      <xdr:row>82</xdr:row>
+      <xdr:row>80</xdr:row>
       <xdr:rowOff>78005</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
       <xdr:colOff>140691</xdr:colOff>
-      <xdr:row>83</xdr:row>
+      <xdr:row>81</xdr:row>
       <xdr:rowOff>83927</xdr:rowOff>
     </xdr:to>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
@@ -4583,13 +4634,13 @@
     <xdr:from>
       <xdr:col>5</xdr:col>
       <xdr:colOff>725616</xdr:colOff>
-      <xdr:row>83</xdr:row>
+      <xdr:row>81</xdr:row>
       <xdr:rowOff>21205</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
       <xdr:colOff>580971</xdr:colOff>
-      <xdr:row>83</xdr:row>
+      <xdr:row>81</xdr:row>
       <xdr:rowOff>26605</xdr:rowOff>
     </xdr:to>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
@@ -4648,13 +4699,13 @@
     <xdr:from>
       <xdr:col>7</xdr:col>
       <xdr:colOff>533103</xdr:colOff>
-      <xdr:row>82</xdr:row>
+      <xdr:row>80</xdr:row>
       <xdr:rowOff>64325</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
       <xdr:colOff>124022</xdr:colOff>
-      <xdr:row>83</xdr:row>
+      <xdr:row>81</xdr:row>
       <xdr:rowOff>27047</xdr:rowOff>
     </xdr:to>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
@@ -4711,150 +4762,20 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>312696</xdr:colOff>
-      <xdr:row>77</xdr:row>
-      <xdr:rowOff>40391</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>532018</xdr:colOff>
-      <xdr:row>78</xdr:row>
-      <xdr:rowOff>58356</xdr:rowOff>
-    </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
-      <mc:Choice Requires="xdr14">
-        <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId25">
-          <xdr14:nvContentPartPr>
-            <xdr14:cNvPr id="13" name="Input penna 12">
-              <a:extLst>
-                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C3AF26A5-F521-4121-B649-97BE2766E13E}"/>
-                </a:ext>
-              </a:extLst>
-            </xdr14:cNvPr>
-            <xdr14:cNvContentPartPr/>
-          </xdr14:nvContentPartPr>
-          <xdr14:nvPr macro=""/>
-          <xdr14:xfrm>
-            <a:off x="5741280" y="13608520"/>
-            <a:ext cx="214560" cy="153082"/>
-          </xdr14:xfrm>
-        </xdr:contentPart>
-      </mc:Choice>
-      <mc:Fallback xmlns="">
-        <xdr:pic>
-          <xdr:nvPicPr>
-            <xdr:cNvPr id="38" name="Input penna 37">
-              <a:extLst>
-                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FEB8E4B5-50AE-0FFA-A532-307F231213C1}"/>
-                </a:ext>
-              </a:extLst>
-            </xdr:cNvPr>
-            <xdr:cNvPicPr/>
-          </xdr:nvPicPr>
-          <xdr:blipFill>
-            <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId26"/>
-            <a:stretch>
-              <a:fillRect/>
-            </a:stretch>
-          </xdr:blipFill>
-          <xdr:spPr>
-            <a:xfrm>
-              <a:off x="5735150" y="13602411"/>
-              <a:ext cx="226821" cy="165300"/>
-            </a:xfrm>
-            <a:prstGeom prst="rect">
-              <a:avLst/>
-            </a:prstGeom>
-          </xdr:spPr>
-        </xdr:pic>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>353059</xdr:colOff>
-      <xdr:row>77</xdr:row>
-      <xdr:rowOff>131553</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>19856</xdr:colOff>
-      <xdr:row>78</xdr:row>
-      <xdr:rowOff>134512</xdr:rowOff>
-    </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
-      <mc:Choice Requires="xdr14">
-        <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId27">
-          <xdr14:nvContentPartPr>
-            <xdr14:cNvPr id="14" name="Input penna 13">
-              <a:extLst>
-                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F9FC48D1-C1E9-42A4-A0B1-2A55CD36FCD5}"/>
-                </a:ext>
-              </a:extLst>
-            </xdr14:cNvPr>
-            <xdr14:cNvContentPartPr/>
-          </xdr14:nvContentPartPr>
-          <xdr14:nvPr macro=""/>
-          <xdr14:xfrm>
-            <a:off x="6867360" y="13699682"/>
-            <a:ext cx="285922" cy="142838"/>
-          </xdr14:xfrm>
-        </xdr:contentPart>
-      </mc:Choice>
-      <mc:Fallback xmlns="">
-        <xdr:pic>
-          <xdr:nvPicPr>
-            <xdr:cNvPr id="47" name="Input penna 46">
-              <a:extLst>
-                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{62A6FE93-BB3B-B427-4F69-A78A5C1F18A0}"/>
-                </a:ext>
-              </a:extLst>
-            </xdr:cNvPr>
-            <xdr:cNvPicPr/>
-          </xdr:nvPicPr>
-          <xdr:blipFill>
-            <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId28"/>
-            <a:stretch>
-              <a:fillRect/>
-            </a:stretch>
-          </xdr:blipFill>
-          <xdr:spPr>
-            <a:xfrm>
-              <a:off x="6861238" y="13693550"/>
-              <a:ext cx="298166" cy="155102"/>
-            </a:xfrm>
-            <a:prstGeom prst="rect">
-              <a:avLst/>
-            </a:prstGeom>
-          </xdr:spPr>
-        </xdr:pic>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
       <xdr:col>6</xdr:col>
       <xdr:colOff>952099</xdr:colOff>
-      <xdr:row>77</xdr:row>
+      <xdr:row>75</xdr:row>
       <xdr:rowOff>132191</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
       <xdr:colOff>430976</xdr:colOff>
-      <xdr:row>78</xdr:row>
-      <xdr:rowOff>58912</xdr:rowOff>
+      <xdr:row>76</xdr:row>
+      <xdr:rowOff>58913</xdr:rowOff>
     </xdr:to>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
       <mc:Choice Requires="xdr14">
-        <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId29">
+        <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId25">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="15" name="Input penna 14">
               <a:extLst>
@@ -4906,132 +4827,63 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>1074499</xdr:colOff>
-      <xdr:row>78</xdr:row>
-      <xdr:rowOff>27593</xdr:rowOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>437984</xdr:colOff>
+      <xdr:row>95</xdr:row>
+      <xdr:rowOff>126556</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>322368</xdr:colOff>
-      <xdr:row>78</xdr:row>
-      <xdr:rowOff>85275</xdr:rowOff>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>442747</xdr:colOff>
+      <xdr:row>96</xdr:row>
+      <xdr:rowOff>131319</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
-      <mc:Choice Requires="xdr14">
-        <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId31">
-          <xdr14:nvContentPartPr>
-            <xdr14:cNvPr id="16" name="Input penna 15">
-              <a:extLst>
-                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3BFA31DA-8520-43EA-ADFD-ABC55E0CD0AC}"/>
-                </a:ext>
-              </a:extLst>
-            </xdr14:cNvPr>
-            <xdr14:cNvContentPartPr/>
-          </xdr14:nvContentPartPr>
-          <xdr14:nvPr macro=""/>
-          <xdr14:xfrm>
-            <a:off x="7588800" y="13735600"/>
-            <a:ext cx="109882" cy="57682"/>
-          </xdr14:xfrm>
-        </xdr:contentPart>
-      </mc:Choice>
-      <mc:Fallback xmlns="">
-        <xdr:pic>
-          <xdr:nvPicPr>
-            <xdr:cNvPr id="53" name="Input penna 52">
-              <a:extLst>
-                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{68B51B8E-16D9-FABA-C418-C0EC26C8837D}"/>
-                </a:ext>
-              </a:extLst>
-            </xdr:cNvPr>
-            <xdr:cNvPicPr/>
-          </xdr:nvPicPr>
-          <xdr:blipFill>
-            <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId32"/>
-            <a:stretch>
-              <a:fillRect/>
-            </a:stretch>
-          </xdr:blipFill>
-          <xdr:spPr>
-            <a:xfrm>
-              <a:off x="7582675" y="13728974"/>
-              <a:ext cx="122131" cy="70933"/>
-            </a:xfrm>
-            <a:prstGeom prst="rect">
-              <a:avLst/>
-            </a:prstGeom>
-          </xdr:spPr>
-        </xdr:pic>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>817225</xdr:colOff>
-      <xdr:row>77</xdr:row>
-      <xdr:rowOff>95831</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>104740</xdr:colOff>
-      <xdr:row>78</xdr:row>
-      <xdr:rowOff>95796</xdr:rowOff>
-    </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
-      <mc:Choice Requires="xdr14">
-        <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId33">
-          <xdr14:nvContentPartPr>
-            <xdr14:cNvPr id="17" name="Input penna 16">
-              <a:extLst>
-                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F8838E0A-9226-4694-A98E-CFA0CE6F0AEE}"/>
-                </a:ext>
-              </a:extLst>
-            </xdr14:cNvPr>
-            <xdr14:cNvContentPartPr/>
-          </xdr14:nvContentPartPr>
-          <xdr14:nvPr macro=""/>
-          <xdr14:xfrm>
-            <a:off x="8417242" y="13663960"/>
-            <a:ext cx="287640" cy="135082"/>
-          </xdr14:xfrm>
-        </xdr:contentPart>
-      </mc:Choice>
-      <mc:Fallback xmlns="">
-        <xdr:pic>
-          <xdr:nvPicPr>
-            <xdr:cNvPr id="58" name="Input penna 57">
-              <a:extLst>
-                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9BACDE61-393A-8FCE-7550-3E6511C8FD26}"/>
-                </a:ext>
-              </a:extLst>
-            </xdr:cNvPr>
-            <xdr:cNvPicPr/>
-          </xdr:nvPicPr>
-          <xdr:blipFill>
-            <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId34"/>
-            <a:stretch>
-              <a:fillRect/>
-            </a:stretch>
-          </xdr:blipFill>
-          <xdr:spPr>
-            <a:xfrm>
-              <a:off x="8411122" y="13657853"/>
-              <a:ext cx="299880" cy="147297"/>
-            </a:xfrm>
-            <a:prstGeom prst="rect">
-              <a:avLst/>
-            </a:prstGeom>
-          </xdr:spPr>
-        </xdr:pic>
-      </mc:Fallback>
-    </mc:AlternateContent>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="19" name="Immagine 18">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9EB4B9AA-92C4-4F37-BD2A-91824047195A}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId31">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="6867360" y="13699682"/>
+          <a:ext cx="1290637" cy="147637"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
@@ -5180,7 +5032,7 @@
   <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="2111.58">13 74 24575,'-1'-1'0,"0"0"0,1 1 0,-1-1 0,0 0 0,0 0 0,0 0 0,1 0 0,-1 0 0,1 0 0,-1 0 0,0 0 0,1 0 0,0 0 0,-1 0 0,1 0 0,0 0 0,-1 0 0,1-1 0,0 1 0,0 0 0,0 0 0,0 0 0,0 0 0,0-1 0,0 1 0,1 0 0,-1-2 0,2 1 0,-1 0 0,0 0 0,1 0 0,-1 0 0,1 0 0,-1 0 0,1 1 0,0-1 0,0 1 0,0-1 0,0 1 0,3-3 0,0 2 0,-1-1 0,0 1 0,1 0 0,0 1 0,-1-1 0,1 1 0,0 0 0,0 0 0,0 0 0,0 0 0,0 1 0,0 0 0,5 0 0,-9 1 0,1 0 0,0-1 0,-1 1 0,1 0 0,-1 0 0,1 0 0,-1 0 0,1 0 0,-1 0 0,1 0 0,-1 1 0,0-1 0,0 0 0,0 1 0,0-1 0,0 1 0,0-1 0,0 1 0,0 0 0,0-1 0,-1 1 0,1 0 0,-1-1 0,1 1 0,-1 0 0,0 0 0,0-1 0,0 1 0,0 0 0,0 0 0,0 0 0,0-1 0,0 1 0,-1 0 0,1 0 0,-1-1 0,1 1 0,-2 2 0,-1 3 0,1 0 0,-1-1 0,0 0 0,-1 1 0,0-1 0,0-2 0,0 2 0,-7 7 0,11-13 0,-1 0 0,1 0 0,-1 1 0,1-1 0,-1 0 0,1 0 0,-1 1 0,1-1 0,-1 0 0,1 1 0,0-1 0,-1 0 0,1 1 0,0-1 0,-1 1 0,1-1 0,0 1 0,0-1 0,-1 0 0,1 1 0,0-1 0,0 1 0,0-1 0,0 1 0,-1-1 0,1 1 0,0-1 0,0 1 0,0 0 0,0-1 0,0 1 0,0-1 0,1 1 0,-1-1 0,0 1 0,0-1 0,0 1 0,0-1 0,1 1 0,-1-1 0,0 0 0,0 1 0,1-1 0,-1 1 0,0-1 0,1 1 0,-1-1 0,0 0 0,1 1 0,-1-1 0,1 0 0,-1 0 0,0 1 0,1-1 0,-1 0 0,1 0 0,-1 1 0,1-1 0,-1 0 0,1 0 0,-1 0 0,1 0 0,-1 0 0,2 0 0,49 5 0,-17-3 0,-33-2 0,0 1 0,0-1 0,-1 0 0,1 1 0,0-1 0,0 1 0,0-1 0,-1 1 0,1-1 0,0 1 0,-1-1 0,1 1 0,0 0 0,-1-1 0,1 1 0,-1 0 0,1 0 0,-1-1 0,1 1 0,-1 0 0,0 0 0,1 0 0,-1 0 0,0-1 0,0 1 0,1 0 0,-1 0 0,0 1 0,-1 0 0,1-1 0,-1 1 0,1-1 0,-1 0 0,0 1 0,0-1 0,1 0 0,-1 1 0,0-1 0,0 0 0,-1 0 0,1 0 0,0 0 0,-2 2 0,-3 1 0,1 0 0,-1-1 0,0 0 0,0 0 0,0 0 0,-13 3 0,-35-2-1365,38-4-5461</inkml:trace>
   <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="4035.77">482 134 24575,'0'-2'0,"-1"0"0,1 0 0,-1 0 0,0 0 0,0 0 0,0 0 0,0 0 0,0 0 0,0 0 0,-1 0 0,1 1 0,-1-1 0,1 1 0,-1-1 0,1 1 0,-1-1 0,0 1 0,0 0 0,-3-1 0,-40-16 0,36 16 0,-1 1 0,1 1 0,-1 0 0,1 0 0,0 0 0,0 1 0,-12 3 0,20-3 0,-1-1 0,0 0 0,1 1 0,-1 0 0,0-1 0,1 1 0,-1 0 0,1 0 0,-1 0 0,1 0 0,-1 0 0,1 0 0,0 1 0,0-1 0,-1 0 0,1 1 0,0-2 0,-1 3 0,2-1 0,0 0 0,-1-1 0,1 1 0,0 0 0,0 0 0,0-1 0,0 1 0,1 0 0,-1 0 0,0 0 0,1-1 0,-1 1 0,1 0 0,0-1 0,-1 1 0,1-1 0,0 1 0,0 0 0,0-1 0,0 0 0,0 1 0,2 1 0,2 1 0,-1 1 0,1-1 0,1 0 0,-1-1 0,0 1 0,1-1 0,0 0 0,-1 0 0,1-1 0,0 0 0,1 0 0,10 2 0,-8-2 0,0 1 0,0 0 0,-1 0 0,16 9 0,-22-11 0,1 1 0,-1 0 0,1 0 0,-1 0 0,0 1 0,0-1 0,0 0 0,0 1 0,-1-1 0,1 1 0,-1 0 0,1-1 0,-1 1 0,0 0 0,0 0 0,0 0 0,-1 0 0,2 5 0,-2-6-3,0-1 0,0 1 0,0-1 0,0 0 0,0 1 0,0-1 0,0 1 0,0-1 0,-1 0 0,1 1 0,0-1 1,-1 0-1,1 1 0,-1-1 0,0 0 0,1 0 0,-1 1 0,0-1 0,0 0 0,0 0 0,1 0 0,-1 0 0,-1 0 0,1 0 0,0 0 0,-2 1 0,-1-1 23,0 0 0,0 1 0,0-1 0,0 0 0,0 0 0,0 0 0,0 0 0,0-1 0,-6 0 0,-2 0-268,-2-1 1,2 0-1,-1-1 1,1 0-1,-18-6 1,9 0-6579</inkml:trace>
   <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="5946.85">662 244 24575,'-1'2'0,"-1"0"0,1 0 0,-1 0 0,0 0 0,1-1 0,-1 1 0,0-1 0,0 1 0,0-1 0,0 0 0,0 1 0,0-1 0,0 0 0,0 0 0,-4 0 0,-11 8 0,15-8 0,0 1 0,1-1 0,-1 0 0,0 1 0,0-1 0,1 1 0,-1 0 0,1-1 0,0 1 0,0 0 0,-1 0 0,1-1 0,0 1 0,0 0 0,1 0 0,-1 0 0,0 0 0,1 1 0,-1-1 0,1 0 0,0 0 0,0 1 0,0-1 0,0 0 0,0 0 0,0 0 0,0 1 0,1-1 0,-1 0 0,1 0 0,0 0 0,0 0 0,0 0 0,0 0 0,0 0 0,0 0 0,0 0 0,2 2 0,0 0 0,1-1 0,-1 1 0,1-1 0,0 0 0,0 0 0,0 0 0,1-1 0,-1 1 0,0-1 0,1 0 0,0 0 0,-1-1 0,1 1 0,0-1 0,0 0 0,6 0 0,-5-1 0,0 0 0,0 0 0,0 0 0,-1-1 0,1 0 0,0 0 0,0-1 0,-1 0 0,1 0 0,-1 0 0,1 0 0,-1-1 0,0 0 0,9-6 0,-12 7 0,0 0 0,0 0 0,0-1 0,0 1 0,-1 0 0,1-1 0,0 1 0,-1-1 0,0 1 0,0-1 0,0 0 0,0 0 0,0 1 0,0-1 0,-1 0 0,1 0 0,-1 0 0,0 0 0,0 0 0,0 0 0,0 0 0,-1 0 0,1 1 0,-1-1 0,1 0 0,-1 1 0,0-1 0,0 1 0,0-1 0,-1 0 0,-2-4 0,-22-24-1365,11 19-5461</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="8803.36">662 244 24575,'3'0'0,"4"0"0,4 0 0,4 0 0,-1 0 0,0 0 0,1-3 0,-2-1-8191</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="8803.35">662 244 24575,'3'0'0,"4"0"0,4 0 0,4 0 0,-1 0 0,0 0 0,1-3 0,-2-1-8191</inkml:trace>
 </inkml:ink>
 </file>
 
@@ -5956,7 +5808,7 @@
           <inkml:channelProperty channel="F" name="resolution" value="0" units="1/dev"/>
         </inkml:channelProperties>
       </inkml:inkSource>
-      <inkml:timestamp xml:id="ts0" timeString="2025-12-17T15:20:04.421"/>
+      <inkml:timestamp xml:id="ts0" timeString="2025-12-17T15:20:04.423"/>
     </inkml:context>
     <inkml:brush xml:id="br0">
       <inkml:brushProperty name="width" value="0.035" units="cm"/>
@@ -5964,8 +5816,9 @@
       <inkml:brushProperty name="color" value="#FFFFFF"/>
     </inkml:brush>
   </inkml:definitions>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0">438 281 24575,'-28'-4'0,"-1"0"0,10-1 0,-10 1 0,12 0 0,-2-1 0,2 0 0,5 1 0,-5-1 0,9 0 0,-3 0 0,2-7 0,-56-18 0,28 19 0,9-1 0,0 0 0,0 0 0,19 0 0,-11 0 0,12 0 0,8-18 0,0 29 0,0 1 0,0 0 0,0 0 0,0-1 0,0 1 0,0 0 0,0 0 0,0-1 0,0 1 0,0 0 0,8-1 0,-8 1 0,0 0 0,0 0 0,0-1 0,0 1 0,0 0 0,0 0 0,12 0 0,-12-1 0,0 1 0,0 0 0,0 0 0,8 0 0,-8-1 0,0 1 0,0 0 0,0 0 0,9 0 0,-9 0 0,0 0 0,0-1 0,8 1 0,-8 0 0,85 6 0,45 13 0,-37-2 0,158 22 0,-129-23 0,90 20 0,-192-33 0,-12 0 0,12-1 0,-3 0 0,2 0 0,-2 0 0,3 0 0,0 0 0,-3 0 0,39 1 0,-47-2 0,2-1 0,-11 1 0,9-1 0,-1 1 0,1-1 0,2 0 0,-11 0 0,8 1 0,1-1 0,2 0 0,-2 0 0,-1 0 0,-8 0 0,9 0 0,2 0 0,-3 0 0,1 0 0,2 0 0,-2 0 0,-9-1 0,8 1 0,1 0 0,2 0 0,-3-1 0,-8 1 0,9-1 0,2 1 0,-11-1 0,9 1 0,-1-1 0,-8 1 0,9-1 0,2 0 0,-11 1 0,8-1 0,-8 0 0,9-1 0,84-17 0,-17 0 0,99-39 0,-118 40 0,-1-1 0,-2 1 0,22 1 0,119-24 0,-195 41 0,0 0 0,0-1 0,9 1 0,-9-1 0,0 1 0,0 0 0,0-1 0,8 1 0,-8 0 0,0-1 0,0 1 0,11 0 0,-11-1 0,0 1 0,9 0 0,-9 0 0,0-1 0,8 1 0,-8 0 0,9 0 0,-9 0 0,0-1 0,11 1 0,-11 0 0,9 0 0,-9 0 0,8 0 0,-8 0 0,0 0 0,11 0 0,-11 0 0,9 0 0,-1 0 0,-8 1 0,9-1 0,2 1 0,-11 0 0,9 0 0,-9-1 0,8 1 0,-8 0 0,11 0 0,-11 0 0,0 0 0,9 0 0,-9-1 0,8 3 0,29 33 0,-26 65 76,-22-50-1517,11-44-5385</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1">3791 178 24575,'48'1'0,"-3"-1"0,3 1 0,-11 0 0,8 0 0,85 4 0,-74-3 0,-8 0 0,6 0 0,87 1 0,-96-3 0,0 1 0,-5 0 0,5 0 0,-8 1 0,11-1 0,-11 1 0,8 1 0,-8-1 0,2 0 0,54 5 0,-84-6 0,-1 0 0,12 0 0,-12 0 0,1 0 0,2 0 0,-11 0 0,9 0 0,-1 1 0,1-1 0,-9 0 0,11 1 0,-3-1 0,-8 0 0,9 1 0,-9-1 0,0 0 0,0 1 0,11-1 0,-11 1 0,0-1 0,0 1 0,0-1 0,0 1 0,-11-1 0,11 1 0,0-1 0,0 0 0,-9 1 0,9-1 0,-8 0 0,-3 1 0,11-1 0,-9 0 0,1 1 0,-1-1 0,-2 0 0,11 0 0,-28 1 0,11 1 0,-11 0 0,-1-1 0,1 1 0,0-1 0,-9 0 0,9 0 0,0 0 0,-9 0 0,9-1 0,-9 1 0,0-1 0,0 0 0,-36 1 0,-198 8 0,347-13 0,-2-1 0,-1 2 0,0-1 0,4 1 0,-4 1 0,12-1 0,-12 1 0,1 1 0,10 0 0,-10 0 0,11 0 0,-12 1 0,114 3 0,-168-4 0,-10 1 0,-1 0 0,12-1 0,-12 1 0,1 0 0,11 0 0,-12 0 0,3 0 0,-2 0 0,-1 0 0,1 0 0,2 0 0,-2 1 0,-1-1 0,3 0 0,-11 1 0,9-1 0,-1 0 0,-8 1 0,9-1 0,-9 1 0,11-1 0,-11 1 0,0-1 0,0 1 0,0-1 0,0 1 0,0-1 0,0 1 0,0 0 0,0-1 0,0 1 0,-11 1 0,2 1 0,1 0 0,-1-1 0,-2 1 0,-6-1 0,6 1 0,-6-1 0,-3 0 0,3 1 0,-3-1 0,1 0 0,2 0 0,-11-1 0,-18 4 0,7-3-91,13-1 0,-13 1 0,2-1 0,0 0 0,1 0 0,-1 0 0,0 0 0,-2-1 0,-7 1 0,10-1 0,-1 0 0,-11-1 0,11 1 0,-64-1 0,27 0-6735</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0">0 213 24575,'1'-4'0,"-1"0"0,1 0 0,0 0 0,0 0 0,1 0 0,-1 0 0,1 0 0,3-6 0,-3 6 0,0 0 0,0-1 0,0 1 0,0-1 0,-1 1 0,1-9 0,-1-3 0,-1-1 0,-1 0 0,-3-18 0,0 5 0,4 29 0,0 0 0,0 0 0,0 0 0,0 0 0,0 0 0,0-1 0,0 1 0,0 0 0,0 0 0,1 0 0,0-2 0,-1 3 0,0 0 0,0 0 0,0 0 0,0-1 0,0 1 0,1 0 0,-1 0 0,0 0 0,0 0 0,0 0 0,0 0 0,1 0 0,-1 0 0,0 0 0,0 0 0,0 0 0,0 0 0,1 0 0,-1 0 0,0 0 0,0 0 0,0 0 0,0 0 0,1 0 0,-1 0 0,0 0 0,0 0 0,0 0 0,0 0 0,1 0 0,-1 0 0,0 0 0,0 0 0,0 1 0,0-1 0,0 0 0,1 0 0,-1 0 0,0 0 0,2 2 0,0 0 0,0 0 0,-1 0 0,1 1 0,-1-1 0,1 0 0,-1 1 0,1 2 0,22 71 0,-22-67 0,2 12 0,1 8 0,-5-27 0,1 0 0,-1-1 0,1 1 0,0-1 0,-1 1 0,1 0 0,0-1 0,0 1 0,0-1 0,0 0 0,0 1 0,2 1 0,-3-3 0,1 0 0,-1 1 0,1-1 0,-1 0 0,1 1 0,-1-1 0,1 0 0,-1 0 0,1 1 0,-1-1 0,1 0 0,-1 0 0,1 0 0,0 0 0,-1 0 0,1 0 0,-1 0 0,1 0 0,-1 0 0,1 0 0,0 0 0,-1 0 0,1 0 0,-1 0 0,1-1 0,-1 1 0,1 0 0,0-1 0,0 0 0,0 0 0,0 0 0,1 0 0,-1 0 0,0 0 0,0-1 0,-1 1 0,1 0 0,0-1 0,1-1 0,1-4 0,0-1 0,3-15 0,-6 22 0,2-4 0,-1-1 0,1 1 0,0 0 0,1-1 0,-1 1 0,1 1 0,0-1 0,1 0 0,-1 1 0,1-1 0,5-4 0,-1-3 0,0 2 0,-6 12 0,-1 8 0,-2 15 0,0-1 0,-9 38 0,7-41-341,0-1 0,2 1-1,1 21 1,0-35-6485</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1">305 241 24575,'0'16'0,"0"-1"0,-1 1 0,-5 22 0,5-34 0,0 0 0,0 0 0,0-1 0,-1 1 0,1 0 0,-1 0 0,0-1 0,0 1 0,0-1 0,-1 0 0,1 0 0,-1 0 0,0 0 0,0 0 0,0 0 0,0 0 0,0-1 0,-7 4 0,5-6 0,7-5 0,9-8 0,50-30 0,-56 39 0,-1 1 0,0 1 0,1-1 0,0 1 0,0 0 0,-1 0 0,1 0 0,0 0 0,1 1 0,-1 0 0,7-1 0,7 1 0,34 1 0,-20 1 0,-31-1-54,0 0-1,0 0 0,0 0 1,0 0-1,-1 0 1,1 1-1,0-1 0,0 1 1,0-1-1,-1 1 1,1 0-1,0-1 0,0 1 1,-1 0-1,1 0 0,-1 0 1,1 0-1,-1 1 1,1-1-1,-1 0 0,0 1 1,0-1-1,1 1 1,0 2-1,2 2-6771</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="2">444 222 24575,'-5'64'0,"0"3"0,6 6-1365,-1-65-5461</inkml:trace>
 </inkml:ink>
 </file>
 
@@ -5985,7 +5838,7 @@
           <inkml:channelProperty channel="F" name="resolution" value="0" units="1/dev"/>
         </inkml:channelProperties>
       </inkml:inkSource>
-      <inkml:timestamp xml:id="ts0" timeString="2025-12-17T15:20:04.423"/>
+      <inkml:timestamp xml:id="ts0" timeString="2025-12-17T15:20:04.426"/>
     </inkml:context>
     <inkml:brush xml:id="br0">
       <inkml:brushProperty name="width" value="0.035" units="cm"/>
@@ -5993,9 +5846,8 @@
       <inkml:brushProperty name="color" value="#FFFFFF"/>
     </inkml:brush>
   </inkml:definitions>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0">0 213 24575,'1'-4'0,"-1"0"0,1 0 0,0 0 0,0 0 0,1 0 0,-1 0 0,1 0 0,3-6 0,-3 6 0,0 0 0,0-1 0,0 1 0,0-1 0,-1 1 0,1-9 0,-1-3 0,-1-1 0,-1 0 0,-3-18 0,0 5 0,4 29 0,0 0 0,0 0 0,0 0 0,0 0 0,0 0 0,0-1 0,0 1 0,0 0 0,0 0 0,1 0 0,0-2 0,-1 3 0,0 0 0,0 0 0,0 0 0,0-1 0,0 1 0,1 0 0,-1 0 0,0 0 0,0 0 0,0 0 0,0 0 0,1 0 0,-1 0 0,0 0 0,0 0 0,0 0 0,0 0 0,1 0 0,-1 0 0,0 0 0,0 0 0,0 0 0,0 0 0,1 0 0,-1 0 0,0 0 0,0 0 0,0 0 0,0 0 0,1 0 0,-1 0 0,0 0 0,0 0 0,0 1 0,0-1 0,0 0 0,1 0 0,-1 0 0,0 0 0,2 2 0,0 0 0,0 0 0,-1 0 0,1 1 0,-1-1 0,1 0 0,-1 1 0,1 2 0,22 71 0,-22-67 0,2 12 0,1 8 0,-5-27 0,1 0 0,-1-1 0,1 1 0,0-1 0,-1 1 0,1 0 0,0-1 0,0 1 0,0-1 0,0 0 0,0 1 0,2 1 0,-3-3 0,1 0 0,-1 1 0,1-1 0,-1 0 0,1 1 0,-1-1 0,1 0 0,-1 0 0,1 1 0,-1-1 0,1 0 0,-1 0 0,1 0 0,0 0 0,-1 0 0,1 0 0,-1 0 0,1 0 0,-1 0 0,1 0 0,0 0 0,-1 0 0,1 0 0,-1 0 0,1-1 0,-1 1 0,1 0 0,0-1 0,0 0 0,0 0 0,0 0 0,1 0 0,-1 0 0,0 0 0,0-1 0,-1 1 0,1 0 0,0-1 0,1-1 0,1-4 0,0-1 0,3-15 0,-6 22 0,2-4 0,-1-1 0,1 1 0,0 0 0,1-1 0,-1 1 0,1 1 0,0-1 0,1 0 0,-1 1 0,1-1 0,5-4 0,-1-3 0,0 2 0,-6 12 0,-1 8 0,-2 15 0,0-1 0,-9 38 0,7-41-341,0-1 0,2 1-1,1 21 1,0-35-6485</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1">305 241 24575,'0'16'0,"0"-1"0,-1 1 0,-5 22 0,5-34 0,0 0 0,0 0 0,0-1 0,-1 1 0,1 0 0,-1 0 0,0-1 0,0 1 0,0-1 0,-1 0 0,1 0 0,-1 0 0,0 0 0,0 0 0,0 0 0,0 0 0,0-1 0,-7 4 0,5-6 0,7-5 0,9-8 0,50-30 0,-56 39 0,-1 1 0,0 1 0,1-1 0,0 1 0,0 0 0,-1 0 0,1 0 0,0 0 0,1 1 0,-1 0 0,7-1 0,7 1 0,34 1 0,-20 1 0,-31-1-54,0 0-1,0 0 0,0 0 1,0 0-1,-1 0 1,1 1-1,0-1 0,0 1 1,0-1-1,-1 1 1,1 0-1,0-1 0,0 1 1,-1 0-1,1 0 0,-1 0 1,1 0-1,-1 1 1,1-1-1,-1 0 0,0 1 1,0-1-1,1 1 1,0 2-1,2 2-6771</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="2">444 222 24575,'-5'64'0,"0"3"0,6 6-1365,-1-65-5461</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0">1 74 24575,'0'4'0,"0"3"0,0 5 0,0 2 0,0 3 0,0 1 0,0 4 0,0 4 0,0 5 0,0-4-8191</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1">14 39 24575,'4'-4'0,"1"0"0,0 1 0,-1-1 0,1 1 0,1 0 0,-1 0 0,0 0 0,1 1 0,0 0 0,-1 0 0,1 1 0,0-1 0,0 1 0,0 1 0,0-1 0,0 1 0,12 0 0,-14 1 0,1-1 0,-1 1 0,0 0 0,0 0 0,0 0 0,0 1 0,0-1 0,0 1 0,-1 0 0,1 0 0,0 0 0,-1 1 0,0-1 0,1 1 0,-1 0 0,0 0 0,0 0 0,-1 0 0,1 0 0,-1 1 0,1-1 0,-1 1 0,0 0 0,-1-1 0,4 8 0,-5-10 0,0 0 0,1 1 0,-1-1 0,0 0 0,1 1 0,-1-1 0,0 1 0,0-1 0,0 0 0,0 1 0,0-1 0,-1 1 0,1-1 0,0 0 0,-1 1 0,1-1 0,-1 0 0,1 1 0,-1-1 0,1 0 0,-1 0 0,0 1 0,0-1 0,0 0 0,0 0 0,0 0 0,0 0 0,0 0 0,0 0 0,0 0 0,0-1 0,0 1 0,-1 0 0,1-1 0,0 1 0,-1-1 0,1 1 0,0-1 0,-1 1 0,1-1 0,0 0 0,-3 0 0,-5 2 0,-1-1 0,0-1 0,1 1 0,-17-3 0,85 48 0,-29-19-1365,-17-14-5461</inkml:trace>
 </inkml:ink>
 </file>
 
@@ -6044,35 +5896,6 @@
           <inkml:channelProperty channel="F" name="resolution" value="0" units="1/dev"/>
         </inkml:channelProperties>
       </inkml:inkSource>
-      <inkml:timestamp xml:id="ts0" timeString="2025-12-17T15:20:04.426"/>
-    </inkml:context>
-    <inkml:brush xml:id="br0">
-      <inkml:brushProperty name="width" value="0.035" units="cm"/>
-      <inkml:brushProperty name="height" value="0.035" units="cm"/>
-      <inkml:brushProperty name="color" value="#FFFFFF"/>
-    </inkml:brush>
-  </inkml:definitions>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0">1 74 24575,'0'4'0,"0"3"0,0 5 0,0 2 0,0 3 0,0 1 0,0 4 0,0 4 0,0 5 0,0-4-8191</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1">14 39 24575,'4'-4'0,"1"0"0,0 1 0,-1-1 0,1 1 0,1 0 0,-1 0 0,0 0 0,1 1 0,0 0 0,-1 0 0,1 1 0,0-1 0,0 1 0,0 1 0,0-1 0,0 1 0,12 0 0,-14 1 0,1-1 0,-1 1 0,0 0 0,0 0 0,0 0 0,0 1 0,0-1 0,0 1 0,-1 0 0,1 0 0,0 0 0,-1 1 0,0-1 0,1 1 0,-1 0 0,0 0 0,0 0 0,-1 0 0,1 0 0,-1 1 0,1-1 0,-1 1 0,0 0 0,-1-1 0,4 8 0,-5-10 0,0 0 0,1 1 0,-1-1 0,0 0 0,1 1 0,-1-1 0,0 1 0,0-1 0,0 0 0,0 1 0,0-1 0,-1 1 0,1-1 0,0 0 0,-1 1 0,1-1 0,-1 0 0,1 1 0,-1-1 0,1 0 0,-1 0 0,0 1 0,0-1 0,0 0 0,0 0 0,0 0 0,0 0 0,0 0 0,0 0 0,0 0 0,0-1 0,0 1 0,-1 0 0,1-1 0,0 1 0,-1-1 0,1 1 0,0-1 0,-1 1 0,1-1 0,0 0 0,-3 0 0,-5 2 0,-1-1 0,0-1 0,1 1 0,-17-3 0,85 48 0,-29-19-1365,-17-14-5461</inkml:trace>
-</inkml:ink>
-</file>
-
-<file path=xl/ink/ink41.xml><?xml version="1.0" encoding="utf-8"?>
-<inkml:ink xmlns:inkml="http://www.w3.org/2003/InkML">
-  <inkml:definitions>
-    <inkml:context xml:id="ctx0">
-      <inkml:inkSource xml:id="inkSrc0">
-        <inkml:traceFormat>
-          <inkml:channel name="X" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
-          <inkml:channel name="Y" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
-          <inkml:channel name="F" type="integer" max="32767" units="dev"/>
-        </inkml:traceFormat>
-        <inkml:channelProperties>
-          <inkml:channelProperty channel="X" name="resolution" value="1000" units="1/cm"/>
-          <inkml:channelProperty channel="Y" name="resolution" value="1000" units="1/cm"/>
-          <inkml:channelProperty channel="F" name="resolution" value="0" units="1/dev"/>
-        </inkml:channelProperties>
-      </inkml:inkSource>
       <inkml:timestamp xml:id="ts0" timeString="2025-12-17T15:20:04.428"/>
     </inkml:context>
     <inkml:brush xml:id="br0">
@@ -6086,7 +5909,7 @@
 </inkml:ink>
 </file>
 
-<file path=xl/ink/ink42.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/ink/ink41.xml><?xml version="1.0" encoding="utf-8"?>
 <inkml:ink xmlns:inkml="http://www.w3.org/2003/InkML">
   <inkml:definitions>
     <inkml:context xml:id="ctx0">
@@ -6114,7 +5937,7 @@
 </inkml:ink>
 </file>
 
-<file path=xl/ink/ink43.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/ink/ink42.xml><?xml version="1.0" encoding="utf-8"?>
 <inkml:ink xmlns:inkml="http://www.w3.org/2003/InkML">
   <inkml:definitions>
     <inkml:context xml:id="ctx0">
@@ -6143,70 +5966,7 @@
 </inkml:ink>
 </file>
 
-<file path=xl/ink/ink44.xml><?xml version="1.0" encoding="utf-8"?>
-<inkml:ink xmlns:inkml="http://www.w3.org/2003/InkML">
-  <inkml:definitions>
-    <inkml:context xml:id="ctx0">
-      <inkml:inkSource xml:id="inkSrc0">
-        <inkml:traceFormat>
-          <inkml:channel name="X" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
-          <inkml:channel name="Y" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
-          <inkml:channel name="F" type="integer" max="32767" units="dev"/>
-        </inkml:traceFormat>
-        <inkml:channelProperties>
-          <inkml:channelProperty channel="X" name="resolution" value="1000" units="1/cm"/>
-          <inkml:channelProperty channel="Y" name="resolution" value="1000" units="1/cm"/>
-          <inkml:channelProperty channel="F" name="resolution" value="0" units="1/dev"/>
-        </inkml:channelProperties>
-      </inkml:inkSource>
-      <inkml:timestamp xml:id="ts0" timeString="2025-12-17T15:20:04.433"/>
-    </inkml:context>
-    <inkml:brush xml:id="br0">
-      <inkml:brushProperty name="width" value="0.035" units="cm"/>
-      <inkml:brushProperty name="height" value="0.035" units="cm"/>
-      <inkml:brushProperty name="color" value="#FFFFFF"/>
-    </inkml:brush>
-  </inkml:definitions>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0">1 242 24575,'0'-8'0,"1"-1"0,0 2 0,1-1 0,0-1 0,0 2 0,0-1 0,1 0 0,0 1 0,2-1 0,-2 0 0,8-9 0,7-9 0,35-39 0,-28 37 0,-25 27 2,1-2-1,0 2 0,0 0 1,0 0-1,-1 0 1,1 0-1,0 0 0,0 0 1,0 0-1,1 1 1,0-2-1,-1 1 1,0 1-1,0-1 0,1 0 1,-1 1-1,0 0 1,0-1-1,1 1 0,-1 0 1,0-1-1,1 1 1,-1 0-1,1 0 0,-1 0 1,0 0-1,1 0 1,-1 1-1,0-1 0,1 0 1,-1 1-1,0-1 1,1 1-1,-1-1 0,0 1 1,0-1-1,0 1 1,0 1-1,1-1 0,-1 0 1,0-1-1,0 1 1,1 0-1,-2 0 0,1 0 1,0 1-1,0-1 1,0 1-1,-1-1 0,1 0 1,-1 1-1,1 1 1,6 12-138,0 2 0,-2-2 1,8 32-1,-6-23-761,-1-2-5929</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1">90 154 24575,'3'0'0,"1"-3"0,4-1 0,3-1 0,3-2 0,3 0 0,0 2 0,2 0 0,1 2 0,-1 2 0,-2-4 0,-5 1-8191</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="2">400 195 24575,'-2'1'0,"0"-1"0,0 1 0,0-1 0,0 1 0,0-1 0,-1 1 0,2 0 0,-1 0 0,0 0 0,0 0 0,1 1 0,-1-1 0,1 1 0,-1-1 0,1 0 0,-1 1 0,1-1 0,0 1 0,0 1 0,0-2 0,0 1 0,0 0 0,0 0 0,0-1 0,0 2 0,1-1 0,-1 0 0,1 0 0,-1 0 0,1 1 0,0-1 0,0 0 0,0 0 0,0 0 0,0 1 0,1 2 0,-1 0 0,0 1 0,0-1 0,1 1 0,0-1 0,0 1 0,0-2 0,0 2 0,1-1 0,0 1 0,0-2 0,0 1 0,0 0 0,6 8 0,-6-12 0,-1 0 0,2 0 0,-2 1 0,0-1 0,0 1 0,1-1 0,-1 1 0,0-1 0,0 0 0,-1 1 0,1-1 0,0 2 0,0-2 0,-1 1 0,1 0 0,-1-1 0,1 1 0,-1-1 0,1 2 0,-1-1 0,0 0 0,0-1 0,0 1 0,0 0 0,0-1 0,-1 2 0,0 2 0,0-4 0,0 1 0,-1 0 0,1-1 0,-1 0 0,0 0 0,1 0 0,-1 0 0,-1-1 0,2 1 0,-1 0 0,0-1 0,0 1 0,0-1 0,0 1 0,1-1 0,-1 0 0,0 0 0,0 0 0,0 0 0,0 0 0,0-1 0,0 1 0,0 0 0,1-1 0,-4-1 0,-27-7-1365,17 5-5461</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="3">570 338 24575,'-15'-1'0,"-1"1"0,0 0 0,-1 0 0,1 2 0,-20 4 0,34-6 0,0 1 0,0-1 0,0 0 0,0 1 0,1-1 0,-1 1 0,0 0 0,0-1 0,1 1 0,-1 0 0,1 0 0,-1 0 0,1 0 0,-2 2 0,2-2 0,-1 0 0,1 1 0,0-1 0,0 0 0,0 1 0,0-1 0,0 2 0,0-1 0,0-1 0,0 1 0,1 0 0,-1 0 0,1 0 0,-1 0 0,1 0 0,-1 0 0,1 0 0,0 1 0,0-1 0,0-1 0,0 1 0,1 0 0,-1 0 0,0 1 0,1-1 0,-1-1 0,1 1 0,0 0 0,-1 0 0,3 3 0,-1-2 0,0 0 0,1 2 0,0-2 0,0 0 0,0-1 0,-1 2 0,1-1 0,1-1 0,-1 0 0,0 1 0,0-1 0,1 0 0,0 0 0,-1-1 0,1 1 0,1 0 0,-2-1 0,1 0 0,0 0 0,0-1 0,0 1 0,0-1 0,0 0 0,0 0 0,0-1 0,5 0 0,-5 1 0,0 0 0,0-1 0,0 1 0,0-1 0,0-1 0,0 1 0,0-1 0,1 1 0,-1-1 0,-1 0 0,1-1 0,-1 1 0,1 0 0,-1-1 0,0 1 0,0-2 0,0 1 0,0 0 0,0 0 0,0-1 0,0 0 0,-1 1 0,0-1 0,0 0 0,2-5 0,-1-9-1365,-2 1-5461</inkml:trace>
-</inkml:ink>
-</file>
-
-<file path=xl/ink/ink45.xml><?xml version="1.0" encoding="utf-8"?>
-<inkml:ink xmlns:inkml="http://www.w3.org/2003/InkML">
-  <inkml:definitions>
-    <inkml:context xml:id="ctx0">
-      <inkml:inkSource xml:id="inkSrc0">
-        <inkml:traceFormat>
-          <inkml:channel name="X" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
-          <inkml:channel name="Y" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
-          <inkml:channel name="F" type="integer" max="32767" units="dev"/>
-        </inkml:traceFormat>
-        <inkml:channelProperties>
-          <inkml:channelProperty channel="X" name="resolution" value="1000" units="1/cm"/>
-          <inkml:channelProperty channel="Y" name="resolution" value="1000" units="1/cm"/>
-          <inkml:channelProperty channel="F" name="resolution" value="0" units="1/dev"/>
-        </inkml:channelProperties>
-      </inkml:inkSource>
-      <inkml:timestamp xml:id="ts0" timeString="2025-12-17T15:20:04.437"/>
-    </inkml:context>
-    <inkml:brush xml:id="br0">
-      <inkml:brushProperty name="width" value="0.035" units="cm"/>
-      <inkml:brushProperty name="height" value="0.035" units="cm"/>
-      <inkml:brushProperty name="color" value="#FFFFFF"/>
-    </inkml:brush>
-  </inkml:definitions>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0">0 76 24575,'23'0'0,"8"3"0,2 4 0,-2 4 0,-16 8 0,-7 2 0,-1 2 0,-7-1 0,0-2-8191</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1">102 76 24575,'-7'-1'0,"-1"0"0,8 1 0,-8-1 0,1 0 0,-1 0 0,-2 0 0,10 0 0,-8 0 0,8 0 0,-8 0 0,1 0 0,7 0 0,0 0 0,-8-1 0,8 1 0,0 0 0,-8 0 0,8-1 0,0 1 0,0 0 0,0 0 0,0 0 0,0 0 0,0-1 0,0 1 0,8 0 0,-8-2 0,15 1 0,-7 0 0,0 0 0,10 0 0,-11 0 0,9 0 0,-9 0 0,9 1 0,-1-1 0,0 1 0,1-1 0,1 1 0,22-4 0,-1 3 0,-7-1 0,2 1 0,5 0 0,1 1 0,-6-1 0,5 1 0,1 0 0,2 0 0,-3 0 0,0 0 0,3 1 0,-3 0 0,42 0 0,-73 1 0,9 0 0,-1-1 0,-7 1 0,7 0 0,-7 0 0,7 0 0,-7 0 0,10 0 0,-11 0 0,9 0 0,-9 1 0,1-1 0,0 0 0,-1 1 0,1-1 0,0 1 0,-1 0 0,1 0 0,0 0 0,-1-1 0,-7 1 0,11 0 0,-11-1 0,7 1 0,-7 0 0,0 0 0,0-1 0,0 1 0,0 0 0,0 0 0,0 0 0,0-1 0,0 1 0,-7 0 0,7 0 0,-11-1 0,11 1 0,-15 2 0,-8 4 0,8-1 0,-8-1 0,0 0 0,-11 1 0,4-1 0,-1 0 0,0 0 0,-56 7 0,87-13 0,-7 0 0,7 0 0,-8 1 0,8-1 0,-8 0 0,8 0 0,-7 1 0,7-1 0,-10 0 0,10 1 0,0-1 0,-8 0 0,8 1 0,0-1 0,-8 1 0,8-1 0,0 1 0,0-1 0,-7 0 0,7 1 0,0-1 0,0 1 0,0-1 0,0 1 0,-8-1 0,8 1 0,0-1 0,0 1 0,0 0 0,0-1 0,0 1 0,0-1 0,8 1 0,-8-1 0,0 1 0,0-1 0,0 1 0,0-1 0,7 2 0,-7-2 0,0 0 0,0 1 0,8-1 0,-8 1 0,0-1 0,8 1 0,-8-1 0,0 0 0,10 1 0,-10-1 0,7 0 0,-7 0 0,0 1 0,8-1 0,-8 0 0,8 0 0,-8 1 0,7-1 0,-7 0 0,8 0 0,-8 0 0,8 0 0,-8 0 0,15 0 0,384 5 0,-131-3 0,-260-2 0,0 1 0,-1-1 0,-7 0 0,8 1 0,0-1 0,-1 1 0,1-1 0,-8 1 0,8-1 0,-1 1 0,-7-1 0,8 1 0,0 0 0,-8-1 0,10 1 0,-10 0 0,8 0 0,-8-1 0,7 1 0,-7 0 0,0 0 0,8 0 0,-8 0 0,0-1 0,0 1 0,8 0 0,-8 0 0,0 1 0,-8 0 0,8-1 0,-8 1 0,8-1 0,-7 1 0,-1 0 0,-2-1 0,10 0 0,-8 1 0,0-1 0,1 0 0,-9 0 0,9 0 0,-1 0 0,-15 2 0,-26 1 0,11 0 0,-8-1 0,-3 0 0,3 0 0,-2 0 0,-100 4 0,-274-3-1365,297-4-5461</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="2">3770 138 24575,'0'-2'0,"-7"0"0,7 0 0,-8 0 0,0 0 0,1 0 0,-1 0 0,0 0 0,1 0 0,-1 0 0,-10 0 0,10 1 0,-7-1 0,7 1 0,-7-1 0,7 1 0,-7-1 0,0 1 0,-1 0 0,-25-3 0,-311-14 0,283 16 0,-3 1 0,1 1 0,-6 0 0,5 0 0,3 0 0,-2 1 0,-93 3 0,154-3 0,-5-1 0,-1 0 0,9 1 0,-9 0 0,1-1 0,7 1 0,-7 0 0,7 0 0,-10 0 0,11 0 0,-9 0 0,9 0 0,-1 1 0,0-1 0,-7 0 0,7 1 0,1 0 0,-9 1 0,16-1 0,0 0 0,-7-1 0,7 1 0,0 0 0,0 0 0,0-1 0,0 1 0,7 0 0,-7 0 0,0 0 0,8-1 0,-8 1 0,8 0 0,-1-1 0,-7 1 0,8-1 0,0 1 0,-1 0 0,1-1 0,0 0 0,-1 2 0,16 0 0,18 1 0,-10 1 0,7-1 0,11 0 0,-11-1 0,0 1 0,11-1 0,-3 0 0,-5 0 0,5-1 0,0 1 0,10-1 0,77 2 0,-69-2 0,5 1 0,3 0 0,-11 0 0,128 9 0,-174-11 0,8 1 0,-7 0 0,9 0 0,-9 0 0,-1 2 0,0-2 0,1 0 0,-1 1 0,-7-1 0,7 1 0,-5 0 0,6-1 0,-9 1 0,1 0 0,0 0 0,-1 0 0,-7 0 0,16 6 0,-16-7-3,0-1 0,0 1 0,0-1 0,0 0 0,0 1 0,0-1 0,0 1 0,0-1 0,-8 0 0,8 1 0,0-1 1,-8 0-1,8 1 0,-7-1 0,-1 0 0,8 0 0,-8 1 0,1-1 0,-1 0 0,0 0 0,8 0 0,-10 0 0,-5 0 0,7 0 0,0 0 0,-15 1 0,-7 0 23,-4 0 0,4 0 0,-1-1 0,0 0 0,-2 0 0,3 0 0,-1 0 0,0-1 0,-48 0 0,-16 0-268,-7-1 1,8 0-1,-6-1 1,5 0-1,-140-8 1,69 2-6579</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="3">5181 251 24575,'-7'2'0,"-9"0"0,9 0 0,-9 0 0,1 0 0,7-1 0,-10 1 0,3 0 0,0 0 0,-1-1 0,1 0 0,0 1 0,-1-1 0,-2 0 0,3 0 0,-31 0 0,-87 8 0,118-8 0,-1 1 0,6-1 0,-5 0 0,0 1 0,-1-1 0,9 1 0,-9 0 0,9-1 0,-1 1 0,0 0 0,-7 0 0,5 1 0,2-1 0,0 0 0,8 0 0,-7 0 0,-1 0 0,8 1 0,-8-1 0,8 0 0,0 0 0,0 1 0,0-1 0,0 0 0,0 0 0,0 0 0,0 1 0,8-1 0,-8 0 0,8 1 0,-1-1 0,1 0 0,0 0 0,2 0 0,-2 0 0,-1 0 0,1 0 0,15 2 0,0 0 0,8-1 0,-6 1 0,6-1 0,-1 0 0,1 0 0,2 1 0,6-2 0,-9 1 0,4-1 0,4 0 0,0 0 0,-7-1 0,10 1 0,-3-1 0,1 0 0,47 0 0,-37-1 0,-3 0 0,0 0 0,3 0 0,-11-1 0,11 0 0,-3 0 0,0-1 0,-6 0 0,6 0 0,-7 0 0,9 0 0,-9-1 0,-1-1 0,72-5 0,-92 7 0,-3 0 0,1 0 0,-1-1 0,0 1 0,-7 0 0,7-1 0,1 1 0,-9-1 0,3 1 0,-2-1 0,0 0 0,-1-1 0,1 2 0,0-1 0,-8 0 0,7 0 0,-7 0 0,0 0 0,0 0 0,0 0 0,0 0 0,-7 0 0,7 1 0,-8-1 0,8 0 0,-8-1 0,1 1 0,-1 1 0,0-1 0,-9 0 0,-14-4 0,-174-25-1365,88 20-5461</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="4">5181 251 24575,'23'0'0,"33"0"0,31 0 0,31 0 0,-11 0 0,3 0 0,8-3 0,-16-1-8191</inkml:trace>
-</inkml:ink>
-</file>
-
-<file path=xl/ink/ink46.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/ink/ink43.xml><?xml version="1.0" encoding="utf-8"?>
 <inkml:ink xmlns:inkml="http://www.w3.org/2003/InkML">
   <inkml:definitions>
     <inkml:context xml:id="ctx0">
@@ -6232,66 +5992,6 @@
   </inkml:definitions>
   <inkml:trace contextRef="#ctx0" brushRef="#br0">456 177 24575,'64'-9'0,"-8"-2"0,1 1 0,1-1 0,46-14 0,189-33 0,-204 43 0,-65 11 0,0-2 0,1 2 0,6 0 0,2 0 0,-8-1 0,48-2 0,-67 6 0,3 1 0,0-1 0,-2 1 0,2 0 0,-9 0 0,9-1 0,-3 1 0,3 0 0,0 0 0,-2 0 0,1 0 0,1 0 0,-2 0 0,-7 0 0,9 0 0,0 0 0,-3 1 0,3-1 0,0 0 0,-2 0 0,-7 1 0,9-1 0,0 1 0,-3-1 0,-6 1 0,9-1 0,-2 1 0,2-1 0,-9 1 0,8 0 0,-8-1 0,7 1 0,2 0 0,-9-1 0,0 1 0,9 1 0,-9-1 0,7 0 0,-7-1 0,0 1 0,0 0 0,8 2 0,130 29-102,-98-22-24,9 0-1,-7 0 1,-11 0 0,2 1-1,-2-1 1,-6 2 0,-8-2 0,8 2-1,-1 18 1,-17-13-6700</inkml:trace>
   <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1">1 139 24575,'24'0'0,"34"0"0,37 0 0,21-3 0,21-2 0,41 1 0,8 0 0,0 2 0,-6 0 0,-2 1 0,-8 0 0,-17-2 0,0-1 0,3 1 0,-34 0-8191</inkml:trace>
-</inkml:ink>
-</file>
-
-<file path=xl/ink/ink47.xml><?xml version="1.0" encoding="utf-8"?>
-<inkml:ink xmlns:inkml="http://www.w3.org/2003/InkML">
-  <inkml:definitions>
-    <inkml:context xml:id="ctx0">
-      <inkml:inkSource xml:id="inkSrc0">
-        <inkml:traceFormat>
-          <inkml:channel name="X" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
-          <inkml:channel name="Y" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
-          <inkml:channel name="F" type="integer" max="32767" units="dev"/>
-        </inkml:traceFormat>
-        <inkml:channelProperties>
-          <inkml:channelProperty channel="X" name="resolution" value="1000" units="1/cm"/>
-          <inkml:channelProperty channel="Y" name="resolution" value="1000" units="1/cm"/>
-          <inkml:channelProperty channel="F" name="resolution" value="0" units="1/dev"/>
-        </inkml:channelProperties>
-      </inkml:inkSource>
-      <inkml:timestamp xml:id="ts0" timeString="2025-12-17T15:20:04.444"/>
-    </inkml:context>
-    <inkml:brush xml:id="br0">
-      <inkml:brushProperty name="width" value="0.035" units="cm"/>
-      <inkml:brushProperty name="height" value="0.035" units="cm"/>
-      <inkml:brushProperty name="color" value="#FFFFFF"/>
-    </inkml:brush>
-  </inkml:definitions>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0">423 38 24575,'-35'1'0,"1"0"0,5 1 0,-5 0 0,1 1 0,3-1 0,-57 7 0,78-7 0,-2-1 0,2 0 0,0 0 0,-2 1 0,2-1 0,0 2 0,-2-2 0,6 1 0,-4 0 0,-11 3 0,20-3 0,0-2 0,-4 1 0,4 0 0,0 0 0,0-1 0,0 1 0,0 0 0,-5 0 0,5-1 0,0 1 0,0 0 0,5 0 0,-5-1 0,0 1 0,0 0 0,0 1 0,0-1 0,4-1 0,-4 1 0,0 0 0,5-1 0,-5 1 0,0 0 0,4-1 0,-4 1 0,7 0 0,-7-1 0,4 1 0,-4-1 0,5 1 0,-1 0 0,12 2 0,-3-1 0,3 0 0,-3-1 0,8 1 0,-8-1 0,3 0 0,2 0 0,31 3 0,-33-4 0,-3 1 0,3-1 0,-7 1 0,4 0 0,3 0 0,-3 0 0,-1 1 0,1-1 0,-2 2 0,3-2 0,-5 1 0,26 4 0,-35-6 0,0 0 0,0 0 0,5 0 0,-5 2 0,0-2 0,0 0 0,0 0 0,0 0 0,0 1 0,0-1 0,4 0 0,-4 0 0,0 1 0,0-1 0,0 0 0,0 0 0,0 1 0,0-1 0,0 0 0,0 0 0,0 1 0,0-1 0,0 0 0,0 0 0,0 0 0,-4 1 0,4-1 0,0 0 0,0 0 0,0 1 0,0-1 0,0 0 0,0 0 0,0 0 0,-5 1 0,5-1 0,0 0 0,0 0 0,0 0 0,-6 0 0,6 0 0,0 1 0,-5-1 0,-71 6 0,-81-3 0,65-3-1365,5 0-5461</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1">936 38 24575,'5'9'0,"2"-1"0,2 1 0,0 0 0,2-1 0,2 0 0,3 1 0,-3-1 0,41 13 0,-49-20 0,-1 2 0,0-2 0,-4 0 0,7 0 0,-2 0 0,-1 0 0,1 0 0,-1 0 0,7 0 0,-6 0 0,-1 0 0,1 1 0,-1-2 0,7 1 0,-6 0 0,-1-1 0,5 1 0,-4-1 0,6 0 0,-6 1 0,-1-1 0,5 0 0,-2 0 0,2 0 0,4 0 0,-2-1 0,-6 0 0,4 1 0,2-1 0,-2 0 0,-5-2 0,5 2 0,-2 0 0,2 0 0,-4-1 0,3 1 0,-1-1 0,-2 1 0,-1-2 0,5 2 0,2-4 0,7-5 0,2 1 0,1 0 0,-8 0 0,3-1 0,-7 0 0,11-18 0,-16 8-1365,1 3-5461</inkml:trace>
-</inkml:ink>
-</file>
-
-<file path=xl/ink/ink48.xml><?xml version="1.0" encoding="utf-8"?>
-<inkml:ink xmlns:inkml="http://www.w3.org/2003/InkML">
-  <inkml:definitions>
-    <inkml:context xml:id="ctx0">
-      <inkml:inkSource xml:id="inkSrc0">
-        <inkml:traceFormat>
-          <inkml:channel name="X" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
-          <inkml:channel name="Y" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
-          <inkml:channel name="F" type="integer" max="32767" units="dev"/>
-        </inkml:traceFormat>
-        <inkml:channelProperties>
-          <inkml:channelProperty channel="X" name="resolution" value="1000" units="1/cm"/>
-          <inkml:channelProperty channel="Y" name="resolution" value="1000" units="1/cm"/>
-          <inkml:channelProperty channel="F" name="resolution" value="0" units="1/dev"/>
-        </inkml:channelProperties>
-      </inkml:inkSource>
-      <inkml:timestamp xml:id="ts0" timeString="2025-12-17T15:20:04.446"/>
-    </inkml:context>
-    <inkml:brush xml:id="br0">
-      <inkml:brushProperty name="width" value="0.035" units="cm"/>
-      <inkml:brushProperty name="height" value="0.035" units="cm"/>
-      <inkml:brushProperty name="color" value="#FFFFFF"/>
-    </inkml:brush>
-  </inkml:definitions>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0">1 32 24575,'19'3'0,"7"4"0,21 6 0,17-1 0,5 1 0,-10 2 0,-20 2 0,-12 4 0,-7 3 0,5-1 0,19 0 0,9-1 0,-14 1 0,11-3 0,3-3-8191</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1">1 12 24575,'1060'-11'0,"-1041"11"0,1 0 0,-1 0 0,1 0 0,-7 1 0,7 0 0,-1-1 0,1 1 0,-1 0 0,26 3 0,-40-4 0,4 2 0,-4-2 0,-5 1 0,6 0 0,2-1 0,-8 1 0,6 0 0,-1 0 0,-5-1 0,9 1 0,-9 0 0,5 0 0,-5 0 0,0-1 0,6 1 0,-6 0 0,0 0 0,8 0 0,-8 0 0,0 3 0,0-1 0,-8 0 0,2 0 0,1 0 0,-4 0 0,4 1 0,-1-1 0,-2-1 0,-3 1 0,2 0 0,-2-1 0,-3 2 0,0-2 0,3 1 0,-3-1 0,3 0 0,-36 3 0,-11 3 0,-1-1 0,-5 0 0,6-2 0,-98 8 0,-75 7 0,231-20 0,0 0 0,0 0 0,0 0 0,0 0 0,-8 0 0,8 0 0,0 0 0,0 0 0,0 0 0,0 0 0,0 0 0,0 0 0,0 1 0,-6-1 0,6 0 0,0 0 0,0 0 0,0 0 0,0 0 0,0 0 0,0 0 0,0 1 0,0-1 0,0 0 0,0 0 0,0 0 0,0 0 0,0 0 0,0 0 0,0 1 0,0-1 0,0 0 0,0 0 0,0 0 0,0 0 0,0 0 0,0 1 0,0-1 0,0 0 0,0 0 0,0 0 0,0 0 0,0 0 0,0 0 0,0 1 0,0-1 0,0 0 0,0 0 0,0 0 0,0 0 0,6 0 0,-6 0 0,0 0 0,0 0 0,0 1 0,0-1 0,0 0 0,0 0 0,8 0 0,-8 0 0,0 0 0,0 0 0,0 0 0,0 0 0,0 0 0,0 0 0,6 0 0,-6 0 0,0 0 0,122 4 0,137-2 0,52-4 0,374 3 0,-677-1 0,-8 0 0,5 0 0,-5 0 0,6 0 0,-6-1 0,8 1 0,-8 1 0,6-1 0,-6 0 0,6 0 0,-6 0 0,8 0 0,-8 0 0,5 0 0,-5 0 0,6 1 0,-6-1 0,8 0 0,-8 0 0,6 1 0,-6-1 0,0 0 0,5 1 0,-5-1 0,9 2 0,-9-2 0,0 0 0,0 1 0,5-1 0,-5 1 0,0-1 0,6 1 0,-6-1 0,0 1 0,0-1 0,0 1 0,0-1 0,8 2 0,-105 17 0,-190 14 0,-60-4-1365,224-19-5461</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="2">3344 110 24575,'-11'1'0,"-3"1"0,0 0 0,3-1 0,-3 0 0,0 1 0,3 0 0,-8-1 0,5-1 0,0 1 0,-6 0 0,9 0 0,-28 0 0,-19 1 0,13 1 0,7 0 0,-1 2 0,0-2 0,0 1 0,0 0 0,5 2 0,-55 6 0,75-10 0,9 1 0,-9-2 0,8 1 0,-7 0 0,7 0 0,-2 0 0,-3 0 0,2 0 0,4 0 0,5 1 0,-6-1 0,-2 0 0,2 0 0,6 0 0,0 1 0,-5-1 0,5 0 0,0 0 0,0 2 0,0-2 0,0 0 0,0 1 0,5-1 0,-5 0 0,6 0 0,2 1 0,3 3 0,9-3 0,-6-1 0,5 0 0,0 0 0,1 1 0,-1-2 0,1 1 0,-1-1 0,1 0 0,-1 1 0,6-1 0,-5-1 0,-1 1 0,6 0 0,-5-1 0,8 0 0,-9 0 0,31 0 0,-11 0 0,-6 0 0,6 1 0,-8 0 0,8 0 0,-6 1 0,45 2 0,-72-3 0,2-1 0,-2 0 0,-1 0 0,4 1 0,-4-1 0,1 1 0,2-1 0,-2 1 0,-1-1 0,-5 1 0,8 0 0,-2 0 0,0-1 0,-1 1 0,-5 0 0,9 0 0,-4 0 0,-5-1 0,6 1 0,-6 0 0,8 0 0,-8 0 0,6 1 0,-6-1 0,0 0 0,5 0 0,-5 1 0,0-1 0,0 0 0,0 0 0,0 0 0,0 0 0,0 0 0,0 0 0,0 0 0,0 0 0,-5 0 0,5 0 0,0 1 0,-6-1 0,6 0 0,-8 0 0,2 1 0,-8 0 0,3 0 0,-3 0 0,3 0 0,-3 0 0,-5-1 0,5 2 0,-6-2 0,9 0 0,-8 0 0,5 0 0,-6 0 0,1 0 0,-1 0 0,6-1 0,-36 1 0,-325 0-1365,264-1-5461</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="3">3939 280 24575,'6'6'0,"-6"-1"0,8 0 0,-2 1 0,-1-1 0,9 0 0,-8 1 0,8-1 0,0-1 0,-3 1 0,8 0 0,1 0 0,-6-1 0,5 0 0,6 1 0,-5-1 0,-1-1 0,9 1 0,-3-1 0,0 1 0,0-1 0,3 0 0,2 0 0,57 3 0,-68-3 0,1-2 0,-1 0 0,1 0 0,-4 0 0,4 0 0,-1-1 0,9 1 0,-9-1 0,1 0 0,-1 0 0,6 0 0,-5 0 0,-1-1 0,1 1 0,-1-1 0,6 0 0,-5 0 0,-1 0 0,1 0 0,-1 0 0,1-2 0,-6 1 0,5 1 0,1-1 0,-9 0 0,8 0 0,-5 0 0,6-1 0,-7 0 0,-1 0 0,1 1 0,1-1 0,-8 0 0,5 1 0,3-1 0,-8-1 0,13-5 0,0 0-195,1 0 0,-6-1 0,-9 1 0,9-1 0,-8 1 0,2-15 0,-8 7-6631</inkml:trace>
 </inkml:ink>
 </file>
 
@@ -13586,10 +13286,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6894759F-3D2E-4A0B-A951-E5C4D7F4DB62}">
-  <dimension ref="A1:AG72"/>
+  <dimension ref="A1:AG79"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="76" workbookViewId="0">
-      <selection activeCell="A16" sqref="A16"/>
+    <sheetView tabSelected="1" topLeftCell="E43" zoomScale="85" workbookViewId="0">
+      <selection activeCell="K67" sqref="K67"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="18" defaultRowHeight="11.25" customHeight="1" x14ac:dyDescent="0.45"/>
@@ -15063,749 +14763,743 @@
         <v>45</v>
       </c>
       <c r="C49" s="62" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D49" s="63" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E49" s="63" t="s">
-        <v>0</v>
-      </c>
-      <c r="F49" s="63" t="s">
-        <v>0</v>
-      </c>
-      <c r="G49" s="104" t="s">
-        <v>0</v>
-      </c>
-      <c r="H49" s="113" t="s">
-        <v>13</v>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="F49" s="87" t="s">
+        <v>1</v>
+      </c>
+      <c r="G49" s="71"/>
+      <c r="H49" s="63"/>
       <c r="I49" s="67" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J49" s="68" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K49" s="68" t="s">
-        <v>0</v>
-      </c>
-      <c r="L49" s="86" t="s">
-        <v>0</v>
-      </c>
-      <c r="M49" s="115" t="s">
-        <v>0</v>
-      </c>
-      <c r="N49" s="112" t="s">
-        <v>13</v>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="L49" s="115" t="s">
+        <v>1</v>
+      </c>
+      <c r="M49" s="98" t="s">
+        <v>20</v>
+      </c>
+      <c r="N49" s="108"/>
       <c r="O49" s="98" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P49" s="95" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q49" s="95" t="s">
-        <v>0</v>
-      </c>
-      <c r="R49" s="95" t="s">
-        <v>0</v>
-      </c>
-      <c r="S49" s="108" t="s">
-        <v>0</v>
-      </c>
-      <c r="T49" s="80" t="s">
-        <v>13</v>
+        <v>1</v>
+      </c>
+      <c r="R49" s="108" t="s">
+        <v>1</v>
+      </c>
+      <c r="S49" s="110" t="s">
+        <v>20</v>
+      </c>
+      <c r="T49" s="96" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="50" spans="1:20" ht="11.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="B50" s="99" t="s">
+      <c r="B50" s="60" t="s">
         <v>46</v>
       </c>
-      <c r="C50" s="62" t="s">
-        <v>1</v>
-      </c>
-      <c r="D50" s="63" t="s">
-        <v>1</v>
-      </c>
-      <c r="E50" s="63" t="s">
-        <v>1</v>
-      </c>
-      <c r="F50" s="87" t="s">
-        <v>1</v>
-      </c>
-      <c r="G50" s="71"/>
-      <c r="H50" s="63"/>
-      <c r="I50" s="67" t="s">
-        <v>1</v>
-      </c>
-      <c r="J50" s="68" t="s">
-        <v>1</v>
-      </c>
-      <c r="K50" s="68" t="s">
-        <v>1</v>
-      </c>
-      <c r="L50" s="115" t="s">
-        <v>1</v>
-      </c>
-      <c r="M50" s="98" t="s">
-        <v>20</v>
-      </c>
-      <c r="N50" s="108"/>
-      <c r="O50" s="98" t="s">
-        <v>1</v>
-      </c>
-      <c r="P50" s="95" t="s">
-        <v>1</v>
-      </c>
-      <c r="Q50" s="95" t="s">
-        <v>1</v>
-      </c>
-      <c r="R50" s="108" t="s">
-        <v>1</v>
-      </c>
-      <c r="S50" s="110" t="s">
-        <v>20</v>
-      </c>
-      <c r="T50" s="96" t="s">
-        <v>20</v>
+      <c r="C50" s="104"/>
+      <c r="D50" s="98" t="s">
+        <v>2</v>
+      </c>
+      <c r="E50" s="108" t="s">
+        <v>2</v>
+      </c>
+      <c r="F50" s="80" t="s">
+        <v>7</v>
+      </c>
+      <c r="G50" s="100" t="s">
+        <v>9</v>
+      </c>
+      <c r="H50" s="113" t="s">
+        <v>8</v>
+      </c>
+      <c r="I50" s="113" t="s">
+        <v>10</v>
+      </c>
+      <c r="J50" s="110" t="s">
+        <v>2</v>
+      </c>
+      <c r="K50" s="116" t="s">
+        <v>2</v>
+      </c>
+      <c r="L50" s="112" t="s">
+        <v>7</v>
+      </c>
+      <c r="M50" s="112" t="s">
+        <v>9</v>
+      </c>
+      <c r="N50" s="112" t="s">
+        <v>8</v>
+      </c>
+      <c r="O50" s="112" t="s">
+        <v>10</v>
+      </c>
+      <c r="P50" s="98" t="s">
+        <v>2</v>
+      </c>
+      <c r="Q50" s="108" t="s">
+        <v>2</v>
+      </c>
+      <c r="R50" s="111" t="s">
+        <v>7</v>
+      </c>
+      <c r="S50" s="111" t="s">
+        <v>9</v>
+      </c>
+      <c r="T50" s="80" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="51" spans="1:20" ht="11.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B51" s="60" t="s">
         <v>47</v>
       </c>
-      <c r="C51" s="104"/>
-      <c r="D51" s="98" t="s">
-        <v>2</v>
-      </c>
-      <c r="E51" s="108" t="s">
-        <v>2</v>
-      </c>
-      <c r="F51" s="80" t="s">
-        <v>7</v>
-      </c>
-      <c r="G51" s="100" t="s">
-        <v>9</v>
-      </c>
-      <c r="H51" s="113" t="s">
-        <v>8</v>
-      </c>
-      <c r="I51" s="113" t="s">
-        <v>10</v>
-      </c>
-      <c r="J51" s="110" t="s">
-        <v>2</v>
-      </c>
-      <c r="K51" s="116" t="s">
-        <v>2</v>
-      </c>
-      <c r="L51" s="112" t="s">
-        <v>7</v>
-      </c>
-      <c r="M51" s="112" t="s">
-        <v>9</v>
-      </c>
-      <c r="N51" s="112" t="s">
-        <v>8</v>
-      </c>
-      <c r="O51" s="112" t="s">
-        <v>10</v>
-      </c>
-      <c r="P51" s="98" t="s">
-        <v>2</v>
-      </c>
-      <c r="Q51" s="108" t="s">
-        <v>2</v>
-      </c>
-      <c r="R51" s="111" t="s">
-        <v>7</v>
-      </c>
-      <c r="S51" s="111" t="s">
-        <v>9</v>
-      </c>
-      <c r="T51" s="80" t="s">
-        <v>32</v>
+      <c r="C51" s="64"/>
+      <c r="D51" s="64"/>
+      <c r="E51" s="64"/>
+      <c r="F51" s="64"/>
+      <c r="G51" s="64"/>
+      <c r="H51" s="64"/>
+      <c r="I51" s="62" t="s">
+        <v>11</v>
+      </c>
+      <c r="J51" s="104" t="s">
+        <v>11</v>
+      </c>
+      <c r="K51" s="62" t="s">
+        <v>19</v>
+      </c>
+      <c r="L51" s="63" t="s">
+        <v>19</v>
+      </c>
+      <c r="M51" s="104" t="s">
+        <v>19</v>
+      </c>
+      <c r="N51" s="113" t="s">
+        <v>22</v>
+      </c>
+      <c r="O51" s="101" t="s">
+        <v>11</v>
+      </c>
+      <c r="P51" s="107" t="s">
+        <v>11</v>
+      </c>
+      <c r="Q51" s="106" t="s">
+        <v>19</v>
+      </c>
+      <c r="R51" s="102" t="s">
+        <v>19</v>
+      </c>
+      <c r="S51" s="107" t="s">
+        <v>19</v>
+      </c>
+      <c r="T51" s="96" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="52" spans="1:20" ht="11.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B52" s="60" t="s">
         <v>48</v>
       </c>
-      <c r="C52" s="64"/>
-      <c r="D52" s="62" t="s">
+      <c r="C52" s="119"/>
+      <c r="D52" s="119"/>
+      <c r="E52" s="119"/>
+      <c r="F52" s="124"/>
+      <c r="G52" s="119"/>
+      <c r="H52" s="119"/>
+      <c r="I52" s="120"/>
+      <c r="J52" s="62" t="s">
+        <v>12</v>
+      </c>
+      <c r="K52" s="104" t="s">
+        <v>12</v>
+      </c>
+      <c r="L52" s="62" t="s">
+        <v>21</v>
+      </c>
+      <c r="M52" s="63" t="s">
+        <v>21</v>
+      </c>
+      <c r="N52" s="104" t="s">
+        <v>21</v>
+      </c>
+      <c r="O52" s="105"/>
+      <c r="P52" s="103" t="s">
+        <v>12</v>
+      </c>
+      <c r="Q52" s="109" t="s">
+        <v>12</v>
+      </c>
+      <c r="R52" s="103" t="s">
+        <v>21</v>
+      </c>
+      <c r="S52" s="103" t="s">
+        <v>21</v>
+      </c>
+      <c r="T52" s="96" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="53" spans="1:20" ht="11.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="B53" s="91" t="s">
+        <v>51</v>
+      </c>
+      <c r="C53" s="121"/>
+      <c r="D53" s="122"/>
+      <c r="E53" s="123"/>
+      <c r="F53" s="123"/>
+      <c r="G53" s="123"/>
+      <c r="H53" s="123" t="s">
+        <v>13</v>
+      </c>
+      <c r="I53" s="125" t="s">
+        <v>16</v>
+      </c>
+      <c r="J53" s="126" t="s">
+        <v>14</v>
+      </c>
+      <c r="K53" s="126" t="s">
+        <v>17</v>
+      </c>
+      <c r="L53" s="126" t="s">
+        <v>15</v>
+      </c>
+      <c r="M53" s="84" t="s">
+        <v>18</v>
+      </c>
+      <c r="N53" s="123" t="s">
+        <v>13</v>
+      </c>
+      <c r="O53" s="125" t="s">
+        <v>16</v>
+      </c>
+      <c r="P53" s="127" t="s">
+        <v>14</v>
+      </c>
+      <c r="Q53" s="127" t="s">
+        <v>17</v>
+      </c>
+      <c r="R53" s="127" t="s">
+        <v>15</v>
+      </c>
+      <c r="S53" s="84" t="s">
+        <v>18</v>
+      </c>
+      <c r="T53" s="123" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="54" spans="1:20" ht="11.25" customHeight="1" thickTop="1" x14ac:dyDescent="0.45">
+      <c r="B54" s="91" t="s">
+        <v>94</v>
+      </c>
+      <c r="C54" s="91" t="s">
+        <v>0</v>
+      </c>
+      <c r="D54" s="91" t="s">
+        <v>0</v>
+      </c>
+      <c r="E54" s="91" t="s">
+        <v>0</v>
+      </c>
+      <c r="F54" s="91" t="s">
+        <v>0</v>
+      </c>
+      <c r="G54" s="91" t="s">
+        <v>0</v>
+      </c>
+      <c r="H54" s="91"/>
+      <c r="I54" s="91" t="s">
+        <v>0</v>
+      </c>
+      <c r="J54" s="91" t="s">
+        <v>0</v>
+      </c>
+      <c r="K54" s="91" t="s">
+        <v>0</v>
+      </c>
+      <c r="L54" s="91" t="s">
+        <v>0</v>
+      </c>
+      <c r="M54" s="91" t="s">
+        <v>0</v>
+      </c>
+      <c r="N54" s="91"/>
+      <c r="O54" s="91" t="s">
+        <v>0</v>
+      </c>
+      <c r="P54" s="91" t="s">
+        <v>0</v>
+      </c>
+      <c r="Q54" s="91" t="s">
+        <v>0</v>
+      </c>
+      <c r="R54" s="91" t="s">
+        <v>0</v>
+      </c>
+      <c r="S54" s="91" t="s">
+        <v>0</v>
+      </c>
+      <c r="T54" s="91"/>
+    </row>
+    <row r="55" spans="1:20" ht="11.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B55" s="91" t="s">
+        <v>95</v>
+      </c>
+      <c r="C55" s="91"/>
+      <c r="D55" s="91" t="s">
         <v>3</v>
       </c>
-      <c r="E52" s="62" t="s">
+      <c r="E55" s="91" t="s">
         <v>3</v>
       </c>
-      <c r="F52" s="63" t="s">
+      <c r="F55" s="91" t="s">
         <v>3</v>
       </c>
-      <c r="G52" s="63" t="s">
+      <c r="G55" s="91" t="s">
         <v>3</v>
       </c>
-      <c r="H52" s="63" t="s">
+      <c r="H55" s="91" t="s">
         <v>3</v>
       </c>
-      <c r="I52" s="76"/>
-      <c r="J52" s="97" t="s">
+      <c r="I55" s="91"/>
+      <c r="J55" s="91" t="s">
         <v>3</v>
       </c>
-      <c r="K52" s="67" t="s">
+      <c r="K55" s="91" t="s">
         <v>3</v>
       </c>
-      <c r="L52" s="68" t="s">
+      <c r="L55" s="91" t="s">
         <v>3</v>
       </c>
-      <c r="M52" s="68" t="s">
+      <c r="M55" s="91" t="s">
         <v>3</v>
       </c>
-      <c r="N52" s="114" t="s">
+      <c r="N55" s="91" t="s">
         <v>3</v>
       </c>
-      <c r="O52" s="114" t="s">
+      <c r="O55" s="91" t="s">
         <v>3</v>
       </c>
-      <c r="P52" s="98" t="s">
+      <c r="P55" s="91" t="s">
         <v>3</v>
       </c>
-      <c r="Q52" s="98" t="s">
+      <c r="Q55" s="91" t="s">
         <v>3</v>
       </c>
-      <c r="R52" s="98" t="s">
+      <c r="R55" s="91" t="s">
         <v>3</v>
       </c>
-      <c r="S52" s="98" t="s">
+      <c r="S55" s="91" t="s">
         <v>3</v>
       </c>
-      <c r="T52" s="80" t="s">
+      <c r="T55" s="91" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="53" spans="1:20" ht="11.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="B53" s="60" t="s">
-        <v>49</v>
-      </c>
-      <c r="C53" s="64"/>
-      <c r="D53" s="64"/>
-      <c r="E53" s="64"/>
-      <c r="F53" s="64"/>
-      <c r="G53" s="64"/>
-      <c r="H53" s="64"/>
-      <c r="I53" s="62" t="s">
-        <v>11</v>
-      </c>
-      <c r="J53" s="104" t="s">
-        <v>11</v>
-      </c>
-      <c r="K53" s="62" t="s">
-        <v>19</v>
-      </c>
-      <c r="L53" s="63" t="s">
-        <v>19</v>
-      </c>
-      <c r="M53" s="104" t="s">
-        <v>19</v>
-      </c>
-      <c r="N53" s="113" t="s">
-        <v>22</v>
-      </c>
-      <c r="O53" s="101" t="s">
-        <v>11</v>
-      </c>
-      <c r="P53" s="107" t="s">
-        <v>11</v>
-      </c>
-      <c r="Q53" s="106" t="s">
-        <v>19</v>
-      </c>
-      <c r="R53" s="102" t="s">
-        <v>19</v>
-      </c>
-      <c r="S53" s="107" t="s">
-        <v>19</v>
-      </c>
-      <c r="T53" s="96" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="54" spans="1:20" ht="11.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="B54" s="60" t="s">
-        <v>50</v>
-      </c>
-      <c r="C54" s="119"/>
-      <c r="D54" s="119"/>
-      <c r="E54" s="119"/>
-      <c r="F54" s="124"/>
-      <c r="G54" s="119"/>
-      <c r="H54" s="119"/>
-      <c r="I54" s="120" t="s">
-        <v>16</v>
-      </c>
-      <c r="J54" s="62" t="s">
-        <v>12</v>
-      </c>
-      <c r="K54" s="104" t="s">
-        <v>12</v>
-      </c>
-      <c r="L54" s="62" t="s">
-        <v>21</v>
-      </c>
-      <c r="M54" s="63" t="s">
-        <v>21</v>
-      </c>
-      <c r="N54" s="104" t="s">
-        <v>21</v>
-      </c>
-      <c r="O54" s="105" t="s">
-        <v>16</v>
-      </c>
-      <c r="P54" s="103" t="s">
-        <v>12</v>
-      </c>
-      <c r="Q54" s="109" t="s">
-        <v>12</v>
-      </c>
-      <c r="R54" s="103" t="s">
-        <v>21</v>
-      </c>
-      <c r="S54" s="103" t="s">
-        <v>21</v>
-      </c>
-      <c r="T54" s="96" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="55" spans="1:20" ht="11.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="B55" s="91" t="s">
-        <v>51</v>
-      </c>
-      <c r="C55" s="121"/>
-      <c r="D55" s="122"/>
-      <c r="E55" s="123"/>
-      <c r="F55" s="123"/>
-      <c r="G55" s="123"/>
-      <c r="H55" s="123"/>
-      <c r="I55" s="125"/>
-      <c r="J55" s="126" t="s">
-        <v>14</v>
-      </c>
-      <c r="K55" s="126" t="s">
-        <v>17</v>
-      </c>
-      <c r="L55" s="126" t="s">
-        <v>15</v>
-      </c>
-      <c r="M55" s="84" t="s">
-        <v>18</v>
-      </c>
-      <c r="O55" s="118"/>
-      <c r="P55" s="127" t="s">
-        <v>14</v>
-      </c>
-      <c r="Q55" s="127" t="s">
-        <v>17</v>
-      </c>
-      <c r="R55" s="127" t="s">
-        <v>15</v>
-      </c>
-      <c r="S55" s="84" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="56" spans="1:20" ht="11.25" customHeight="1" thickTop="1" x14ac:dyDescent="0.45"/>
-    <row r="57" spans="1:20" ht="11.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A57" t="s">
+    <row r="61" spans="1:20" ht="11.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A61" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="58" spans="1:20" ht="11.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A58" s="89" t="s">
+    <row r="62" spans="1:20" ht="11.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A62" s="89" t="s">
         <v>33</v>
       </c>
-      <c r="B58" s="92" t="s">
+      <c r="B62" s="92" t="s">
+        <v>96</v>
+      </c>
+      <c r="H62" s="93" t="s">
+        <v>96</v>
+      </c>
+      <c r="L62" s="92" t="s">
+        <v>109</v>
+      </c>
+      <c r="M62" s="94" t="s">
+        <v>72</v>
+      </c>
+      <c r="O62" s="93" t="s">
+        <v>96</v>
+      </c>
+      <c r="R62" s="92" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="63" spans="1:20" ht="11.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A63" s="89" t="s">
+        <v>34</v>
+      </c>
+      <c r="C63" s="92" t="s">
+        <v>97</v>
+      </c>
+      <c r="D63" s="92"/>
+      <c r="E63" s="92" t="s">
+        <v>98</v>
+      </c>
+      <c r="F63" s="92" t="s">
+        <v>100</v>
+      </c>
+      <c r="G63" s="92" t="s">
+        <v>99</v>
+      </c>
+      <c r="H63" s="92" t="s">
+        <v>101</v>
+      </c>
+      <c r="I63" s="93" t="s">
+        <v>97</v>
+      </c>
+      <c r="J63" s="93"/>
+      <c r="K63" s="93" t="s">
+        <v>98</v>
+      </c>
+      <c r="L63" s="93" t="s">
+        <v>102</v>
+      </c>
+      <c r="M63" s="93" t="s">
+        <v>99</v>
+      </c>
+      <c r="N63" s="93" t="s">
+        <v>101</v>
+      </c>
+      <c r="P63" s="93" t="s">
+        <v>97</v>
+      </c>
+      <c r="Q63" s="93" t="s">
+        <v>98</v>
+      </c>
+      <c r="R63" s="93" t="s">
+        <v>102</v>
+      </c>
+      <c r="S63" s="93" t="s">
+        <v>99</v>
+      </c>
+      <c r="T63" s="93" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="64" spans="1:20" ht="11.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A64" s="89" t="s">
+        <v>35</v>
+      </c>
+      <c r="F64" s="88"/>
+      <c r="H64" s="92" t="s">
+        <v>105</v>
+      </c>
+      <c r="I64" s="92" t="s">
+        <v>107</v>
+      </c>
+      <c r="J64" s="92" t="s">
+        <v>106</v>
+      </c>
+      <c r="K64" s="92" t="s">
+        <v>108</v>
+      </c>
+      <c r="M64" s="92" t="s">
+        <v>110</v>
+      </c>
+      <c r="N64" s="93" t="s">
+        <v>105</v>
+      </c>
+      <c r="O64" s="92" t="s">
+        <v>107</v>
+      </c>
+      <c r="P64" s="92" t="s">
+        <v>106</v>
+      </c>
+      <c r="Q64" s="92" t="s">
+        <v>108</v>
+      </c>
+      <c r="S64" s="92" t="s">
+        <v>110</v>
+      </c>
+      <c r="T64" s="93" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="67" spans="1:20" ht="11.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="G67" s="128" t="s">
+        <v>103</v>
+      </c>
+      <c r="H67" s="128" t="s">
+        <v>128</v>
+      </c>
+      <c r="I67" s="128" t="s">
+        <v>129</v>
+      </c>
+      <c r="K67" s="88"/>
+      <c r="N67" s="128" t="s">
+        <v>104</v>
+      </c>
+      <c r="O67" s="128" t="s">
         <v>41</v>
       </c>
-      <c r="C58" s="92" t="s">
+      <c r="P67" s="128" t="s">
         <v>43</v>
       </c>
-      <c r="D58" s="92"/>
-      <c r="E58" s="92" t="s">
-        <v>52</v>
-      </c>
-      <c r="F58" s="92" t="s">
-        <v>53</v>
-      </c>
-      <c r="G58" s="92" t="s">
-        <v>54</v>
-      </c>
-      <c r="H58" s="92" t="s">
-        <v>56</v>
-      </c>
-      <c r="I58" s="93" t="s">
-        <v>43</v>
-      </c>
-      <c r="J58" s="93"/>
-      <c r="K58" s="93" t="s">
-        <v>52</v>
-      </c>
-      <c r="L58" s="93" t="s">
-        <v>53</v>
-      </c>
-      <c r="M58" s="93" t="s">
-        <v>54</v>
-      </c>
-      <c r="N58" s="93" t="s">
-        <v>56</v>
-      </c>
-      <c r="O58" s="93" t="s">
-        <v>41</v>
-      </c>
-      <c r="P58" s="93" t="s">
-        <v>43</v>
-      </c>
-      <c r="Q58" s="93" t="s">
-        <v>52</v>
-      </c>
-      <c r="R58" s="93" t="s">
-        <v>53</v>
-      </c>
-      <c r="S58" s="93" t="s">
-        <v>54</v>
-      </c>
-      <c r="T58" s="93" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="59" spans="1:20" ht="11.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A59" s="89" t="s">
-        <v>34</v>
-      </c>
-      <c r="B59" s="92" t="s">
-        <v>42</v>
-      </c>
-      <c r="C59" s="92" t="s">
-        <v>44</v>
-      </c>
-      <c r="D59" s="92"/>
-      <c r="E59" s="92"/>
-      <c r="F59" s="92"/>
-      <c r="G59" s="92" t="s">
+      <c r="S67" s="129" t="s">
         <v>72</v>
       </c>
-      <c r="H59" s="92" t="s">
-        <v>73</v>
-      </c>
-      <c r="I59" s="93" t="s">
-        <v>44</v>
-      </c>
-      <c r="J59" s="93"/>
-      <c r="K59" s="93"/>
-      <c r="L59" s="93"/>
-      <c r="M59" s="94" t="s">
-        <v>72</v>
-      </c>
-      <c r="N59" s="93" t="s">
-        <v>73</v>
-      </c>
-      <c r="O59" s="93" t="s">
-        <v>42</v>
-      </c>
-      <c r="P59" s="93" t="s">
-        <v>44</v>
-      </c>
-      <c r="Q59" s="93"/>
-      <c r="R59" s="93"/>
-      <c r="S59" s="94" t="s">
-        <v>55</v>
-      </c>
-      <c r="T59" s="93" t="s">
+      <c r="T67" s="128" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="60" spans="1:20" ht="11.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A60" s="89" t="s">
-        <v>35</v>
-      </c>
-      <c r="F60" s="88"/>
-      <c r="H60" s="92" t="s">
-        <v>58</v>
-      </c>
-      <c r="I60" s="92" t="s">
-        <v>59</v>
-      </c>
-      <c r="J60" s="92" t="s">
-        <v>60</v>
-      </c>
-      <c r="K60" s="92" t="s">
-        <v>61</v>
-      </c>
-      <c r="L60" s="92" t="s">
-        <v>62</v>
-      </c>
-      <c r="M60" s="92" t="s">
-        <v>63</v>
-      </c>
-      <c r="N60" s="93" t="s">
-        <v>58</v>
-      </c>
-      <c r="O60" s="92" t="s">
-        <v>59</v>
-      </c>
-      <c r="P60" s="92" t="s">
-        <v>60</v>
-      </c>
-      <c r="Q60" s="92" t="s">
-        <v>61</v>
-      </c>
-      <c r="R60" s="92" t="s">
-        <v>62</v>
-      </c>
-      <c r="S60" s="92" t="s">
-        <v>63</v>
-      </c>
-      <c r="T60" s="93" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="61" spans="1:20" ht="11.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A61" s="89" t="s">
-        <v>36</v>
-      </c>
-      <c r="H61" s="93" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="62" spans="1:20" ht="11.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="H62" s="93" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="66" spans="1:20" ht="11.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A66" s="90" t="s">
+    <row r="68" spans="1:20" ht="11.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="H68" s="128" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="70" spans="1:20" ht="11.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A70" s="90" t="s">
         <v>37</v>
       </c>
-      <c r="C66" s="92" t="s">
-        <v>82</v>
-      </c>
-      <c r="D66" s="92" t="s">
-        <v>83</v>
-      </c>
-      <c r="E66" s="92" t="s">
-        <v>67</v>
-      </c>
-      <c r="F66" s="92" t="s">
-        <v>74</v>
-      </c>
-      <c r="G66" s="92" t="s">
+      <c r="C70" s="92" t="s">
+        <v>111</v>
+      </c>
+      <c r="D70" s="92" t="s">
+        <v>112</v>
+      </c>
+      <c r="E70" s="92" t="s">
+        <v>113</v>
+      </c>
+      <c r="F70" s="92" t="s">
+        <v>118</v>
+      </c>
+      <c r="I70" s="93" t="s">
+        <v>111</v>
+      </c>
+      <c r="J70" s="93" t="s">
+        <v>112</v>
+      </c>
+      <c r="K70" s="93" t="s">
+        <v>113</v>
+      </c>
+      <c r="L70" s="93" t="s">
+        <v>118</v>
+      </c>
+      <c r="N70" s="93" t="s">
+        <v>114</v>
+      </c>
+      <c r="O70" s="92" t="s">
+        <v>111</v>
+      </c>
+      <c r="P70" s="92" t="s">
+        <v>112</v>
+      </c>
+      <c r="Q70" s="92" t="s">
+        <v>113</v>
+      </c>
+      <c r="R70" s="92" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="71" spans="1:20" ht="11.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A71" s="90" t="s">
+        <v>38</v>
+      </c>
+      <c r="C71" s="92" t="s">
+        <v>68</v>
+      </c>
+      <c r="D71" s="92" t="s">
+        <v>69</v>
+      </c>
+      <c r="E71" s="92" t="s">
+        <v>70</v>
+      </c>
+      <c r="G71" s="88"/>
+      <c r="H71" s="92" t="s">
+        <v>114</v>
+      </c>
+      <c r="I71" s="92" t="s">
+        <v>115</v>
+      </c>
+      <c r="J71" s="92" t="s">
+        <v>116</v>
+      </c>
+      <c r="K71" s="92" t="s">
+        <v>117</v>
+      </c>
+      <c r="L71" s="93" t="s">
+        <v>119</v>
+      </c>
+      <c r="M71" s="92" t="s">
+        <v>120</v>
+      </c>
+      <c r="N71" s="92" t="s">
+        <v>122</v>
+      </c>
+      <c r="O71" s="92" t="s">
+        <v>68</v>
+      </c>
+      <c r="P71" s="92" t="s">
+        <v>69</v>
+      </c>
+      <c r="Q71" s="92" t="s">
+        <v>70</v>
+      </c>
+      <c r="S71" s="88"/>
+      <c r="T71" s="92" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="72" spans="1:20" ht="11.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A72" s="90" t="s">
+        <v>39</v>
+      </c>
+      <c r="F72" s="92" t="s">
+        <v>119</v>
+      </c>
+      <c r="M72" s="92" t="s">
+        <v>121</v>
+      </c>
+      <c r="N72" s="92" t="s">
+        <v>123</v>
+      </c>
+      <c r="O72" s="93" t="s">
+        <v>115</v>
+      </c>
+      <c r="P72" s="93" t="s">
+        <v>116</v>
+      </c>
+      <c r="Q72" s="93" t="s">
+        <v>117</v>
+      </c>
+      <c r="R72" s="92" t="s">
+        <v>119</v>
+      </c>
+      <c r="S72" s="93" t="s">
+        <v>120</v>
+      </c>
+      <c r="T72" s="93" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="73" spans="1:20" ht="11.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A73" s="90" t="s">
+        <v>40</v>
+      </c>
+      <c r="F73" s="92" t="s">
+        <v>70</v>
+      </c>
+      <c r="I73" s="128" t="s">
+        <v>125</v>
+      </c>
+      <c r="J73" s="128" t="s">
+        <v>126</v>
+      </c>
+      <c r="K73" s="128" t="s">
+        <v>127</v>
+      </c>
+      <c r="N73" s="128" t="s">
+        <v>124</v>
+      </c>
+      <c r="S73" s="93" t="s">
+        <v>121</v>
+      </c>
+      <c r="T73" s="93" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="75" spans="1:20" ht="11.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="J75" t="s">
+        <v>89</v>
+      </c>
+      <c r="K75" t="s">
+        <v>89</v>
+      </c>
+      <c r="L75" t="s">
+        <v>88</v>
+      </c>
+      <c r="P75" t="s">
+        <v>89</v>
+      </c>
+      <c r="Q75" t="s">
+        <v>89</v>
+      </c>
+      <c r="R75" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="76" spans="1:20" ht="11.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="M76" t="s">
+        <v>88</v>
+      </c>
+      <c r="S76" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="77" spans="1:20" ht="11.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="F77" s="128" t="s">
+        <v>75</v>
+      </c>
+      <c r="G77" s="128" t="s">
         <v>77</v>
       </c>
-      <c r="H66" s="92" t="s">
+      <c r="H77" s="128" t="s">
+        <v>80</v>
+      </c>
+      <c r="L77" s="128" t="s">
+        <v>75</v>
+      </c>
+      <c r="M77" s="128" t="s">
+        <v>77</v>
+      </c>
+      <c r="N77" s="128" t="s">
+        <v>80</v>
+      </c>
+      <c r="O77" s="128" t="s">
+        <v>84</v>
+      </c>
+      <c r="R77" s="128" t="s">
+        <v>75</v>
+      </c>
+      <c r="S77" s="128" t="s">
+        <v>77</v>
+      </c>
+      <c r="T77" s="128" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="78" spans="1:20" ht="11.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="H78" s="128" t="s">
         <v>79</v>
       </c>
-      <c r="I66" s="93" t="s">
-        <v>82</v>
-      </c>
-      <c r="J66" s="93" t="s">
-        <v>83</v>
-      </c>
-      <c r="K66" s="93" t="s">
-        <v>67</v>
-      </c>
-      <c r="L66" s="93" t="s">
-        <v>74</v>
-      </c>
-      <c r="M66" s="93" t="s">
-        <v>77</v>
-      </c>
-      <c r="N66" s="93" t="s">
+      <c r="T78" s="128" t="s">
         <v>79</v>
       </c>
-      <c r="O66" s="92" t="s">
-        <v>82</v>
-      </c>
-      <c r="P66" s="92" t="s">
-        <v>83</v>
-      </c>
-      <c r="Q66" s="92" t="s">
-        <v>67</v>
-      </c>
-      <c r="R66" s="92" t="s">
-        <v>74</v>
-      </c>
-      <c r="S66" s="92" t="s">
-        <v>77</v>
-      </c>
-      <c r="T66" s="92" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="67" spans="1:20" ht="11.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A67" s="90" t="s">
-        <v>38</v>
-      </c>
-      <c r="C67" s="92" t="s">
+    </row>
+    <row r="79" spans="1:20" ht="11.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="I79" s="93" t="s">
         <v>68</v>
       </c>
-      <c r="D67" s="92" t="s">
+      <c r="J79" s="93" t="s">
         <v>69</v>
       </c>
-      <c r="E67" s="92" t="s">
+      <c r="K79" s="93" t="s">
         <v>70</v>
       </c>
-      <c r="F67" s="92" t="s">
-        <v>75</v>
-      </c>
-      <c r="G67" s="88"/>
-      <c r="H67" s="92" t="s">
-        <v>78</v>
-      </c>
-      <c r="I67" s="93" t="s">
-        <v>68</v>
-      </c>
-      <c r="J67" s="93" t="s">
-        <v>69</v>
-      </c>
-      <c r="K67" s="93" t="s">
+      <c r="L79" s="93" t="s">
         <v>70</v>
       </c>
-      <c r="L67" s="93" t="s">
-        <v>75</v>
-      </c>
-      <c r="M67" s="88"/>
-      <c r="N67" s="93" t="s">
-        <v>78</v>
-      </c>
-      <c r="O67" s="92" t="s">
-        <v>68</v>
-      </c>
-      <c r="P67" s="92" t="s">
-        <v>69</v>
-      </c>
-      <c r="Q67" s="92" t="s">
+      <c r="R79" s="92" t="s">
         <v>70</v>
-      </c>
-      <c r="R67" s="92" t="s">
-        <v>75</v>
-      </c>
-      <c r="S67" s="88"/>
-      <c r="T67" s="92" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="68" spans="1:20" ht="11.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A68" s="90" t="s">
-        <v>39</v>
-      </c>
-      <c r="F68" s="92" t="s">
-        <v>76</v>
-      </c>
-      <c r="H68" s="92" t="s">
-        <v>80</v>
-      </c>
-      <c r="L68" s="93" t="s">
-        <v>76</v>
-      </c>
-      <c r="N68" s="93" t="s">
-        <v>80</v>
-      </c>
-      <c r="R68" s="92" t="s">
-        <v>76</v>
-      </c>
-      <c r="T68" s="92" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="69" spans="1:20" ht="11.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A69" s="90" t="s">
-        <v>40</v>
-      </c>
-      <c r="F69" s="92" t="s">
-        <v>70</v>
-      </c>
-      <c r="L69" s="93" t="s">
-        <v>70</v>
-      </c>
-      <c r="R69" s="92" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="70" spans="1:20" ht="11.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="I70" s="92" t="s">
-        <v>84</v>
-      </c>
-      <c r="J70" s="92" t="s">
-        <v>86</v>
-      </c>
-      <c r="K70" s="92" t="s">
-        <v>87</v>
-      </c>
-      <c r="M70" s="92" t="s">
-        <v>90</v>
-      </c>
-      <c r="N70" s="92" t="s">
-        <v>92</v>
-      </c>
-      <c r="O70" s="93" t="s">
-        <v>84</v>
-      </c>
-      <c r="P70" s="93" t="s">
-        <v>86</v>
-      </c>
-      <c r="Q70" s="93" t="s">
-        <v>87</v>
-      </c>
-      <c r="S70" s="93" t="s">
-        <v>90</v>
-      </c>
-      <c r="T70" s="93" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="71" spans="1:20" ht="11.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="I71" s="92" t="s">
-        <v>85</v>
-      </c>
-      <c r="J71" t="s">
-        <v>89</v>
-      </c>
-      <c r="K71" t="s">
-        <v>89</v>
-      </c>
-      <c r="L71" t="s">
-        <v>88</v>
-      </c>
-      <c r="M71" s="92" t="s">
-        <v>91</v>
-      </c>
-      <c r="N71" s="92" t="s">
-        <v>93</v>
-      </c>
-      <c r="O71" s="93" t="s">
-        <v>85</v>
-      </c>
-      <c r="P71" t="s">
-        <v>89</v>
-      </c>
-      <c r="Q71" t="s">
-        <v>89</v>
-      </c>
-      <c r="R71" t="s">
-        <v>88</v>
-      </c>
-      <c r="S71" s="93" t="s">
-        <v>91</v>
-      </c>
-      <c r="T71" s="93" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="72" spans="1:20" ht="11.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="M72" t="s">
-        <v>88</v>
-      </c>
-      <c r="S72" t="s">
-        <v>88</v>
       </c>
     </row>
   </sheetData>

</xml_diff>